<commit_message>
ActionClass change in OpenURL
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\Run1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B51D7D-B3FF-4721-AA4E-3EADC1D71BC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{5E3BCD27-1CE0-45F8-AD5E-79BBC0639395}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="3" firstSheet="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="DriverSheet" sheetId="2" r:id="rId2"/>
-    <sheet name="VerifyCSVForExistingVersion" sheetId="3" r:id="rId3"/>
-    <sheet name="VerifyCSVForNewVersion" sheetId="4" r:id="rId4"/>
-    <sheet name="VerifyDeleteOffer" sheetId="5" r:id="rId5"/>
-    <sheet name="VerifyEventAPI" sheetId="6" r:id="rId6"/>
-    <sheet name="Cases_RealTimeSpine" sheetId="7" r:id="rId7"/>
-    <sheet name="BatchDecisionOutputValidations" sheetId="8" r:id="rId8"/>
-    <sheet name="CheckLists" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="DriverSheet" r:id="rId2" sheetId="2"/>
+    <sheet name="VerifyCSVForExistingVersion" r:id="rId3" sheetId="3"/>
+    <sheet name="VerifyCSVForNewVersion" r:id="rId4" sheetId="4"/>
+    <sheet name="VerifyDeleteOffer" r:id="rId5" sheetId="5"/>
+    <sheet name="VerifyEventAPI" r:id="rId6" sheetId="6"/>
+    <sheet name="Cases_RealTimeSpine" r:id="rId7" sheetId="7"/>
+    <sheet name="BatchDecisionOutputValidations" r:id="rId8" sheetId="8"/>
+    <sheet name="CheckLists" r:id="rId9" sheetId="9"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="294">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -906,6 +906,9 @@
   </si>
   <si>
     <t>Deselect web</t>
+  </si>
+  <si>
+    <t>uncheck cc</t>
   </si>
   <si>
     <t>Pass</t>
@@ -1093,58 +1096,58 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1225,7 +1228,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1277,10 +1280,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1315,7 +1318,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1367,7 +1370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1478,21 +1481,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1509,7 +1512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1561,23 +1564,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1601,31 +1604,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.42578125" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="1025" width="9.140625" style="2" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="70.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="24.42578125" collapsed="true"/>
+    <col min="6" max="1025" customWidth="true" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="1" s="3" spans="1:5">
       <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
@@ -1634,7 +1637,7 @@
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="2" s="3" spans="1:5">
       <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
@@ -1643,14 +1646,14 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="3" s="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="4" s="6" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1747,29 +1750,29 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMK47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="D40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1852,9 +1855,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -1876,9 +1877,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -1900,9 +1899,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -1922,9 +1919,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1946,9 +1941,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -1968,9 +1961,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -1992,9 +1983,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -2014,9 +2003,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -2038,9 +2025,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -2060,9 +2045,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -2084,9 +2067,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -2108,9 +2089,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -2132,9 +2111,7 @@
         <v>68</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="11" t="s">
@@ -2156,9 +2133,7 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
@@ -2178,9 +2153,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="11" t="s">
@@ -2202,9 +2175,7 @@
         <v>76</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="11" t="s">
@@ -2226,9 +2197,7 @@
         <v>80</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="11" t="s">
@@ -2248,9 +2217,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="11" t="s">
@@ -2272,9 +2239,7 @@
         <v>3000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="11" t="s">
@@ -2294,9 +2259,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="11" t="s">
@@ -2316,9 +2279,7 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="11" t="s">
@@ -2338,9 +2299,7 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="11" t="s">
@@ -2360,9 +2319,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="11" t="s">
@@ -2382,9 +2339,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="11" t="s">
@@ -2404,9 +2359,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="19" t="s">
@@ -2426,9 +2379,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="11" t="s">
@@ -2448,9 +2399,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="11" t="s">
@@ -2472,9 +2421,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="11" t="s">
@@ -2494,9 +2441,7 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="11" t="s">
@@ -2518,9 +2463,7 @@
         <v>3000</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="11" t="s">
@@ -2540,9 +2483,7 @@
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="11" t="s">
@@ -2564,9 +2505,7 @@
         <v>3000</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="11" t="s">
@@ -2586,9 +2525,7 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="11" t="s">
@@ -2608,9 +2545,7 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="11" t="s">
@@ -2632,9 +2567,7 @@
         <v>20000</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="11" t="s">
@@ -2654,9 +2587,7 @@
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="11" t="s">
@@ -2676,9 +2607,7 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="11" t="s">
@@ -2698,9 +2627,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="11" t="s">
@@ -2722,9 +2649,7 @@
         <v>10000</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="11" t="s">
@@ -2744,9 +2669,7 @@
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="11" t="s">
@@ -2766,9 +2689,7 @@
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="11" t="s">
@@ -2790,9 +2711,7 @@
         <v>30000</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="11" t="s">
@@ -2812,9 +2731,7 @@
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H47" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2822,28 +2739,28 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="7" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2926,7 +2843,9 @@
         <v>38</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -2948,7 +2867,9 @@
         <v>38</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -2970,7 +2891,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -2990,7 +2913,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -3012,7 +2937,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -3032,7 +2959,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -3054,7 +2983,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -3074,7 +3005,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -3096,7 +3029,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -3116,7 +3051,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -3138,7 +3075,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -3160,7 +3099,9 @@
         <v>64</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -3182,7 +3123,9 @@
         <v>68</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -3202,7 +3145,9 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -3224,7 +3169,9 @@
         <v>131</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -3246,7 +3193,9 @@
         <v>80</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -3266,7 +3215,9 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="9"/>
+      <c r="H21" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -3288,7 +3239,9 @@
         <v>3000</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -3308,7 +3261,9 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -3328,7 +3283,9 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="H24" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -3348,7 +3305,9 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -3368,7 +3327,9 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -3378,487 +3339,531 @@
         <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>137</v>
+        <v>291</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="9"/>
+        <v>93</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>49</v>
+        <v>136</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>142</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F32" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="13">
-        <v>43525</v>
-      </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="13">
-        <v>45743</v>
-      </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F35" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="H35" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>142</v>
+      </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="H36" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F37" s="13">
+        <v>43525</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F38" s="13">
+        <v>45743</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G39" s="1"/>
-      <c r="H39" s="9"/>
+        <v>49</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F41" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+        <v>154</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>83</v>
+        <v>157</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="9">
-        <v>10000</v>
-      </c>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+        <v>154</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F45" s="9">
+        <v>5000</v>
+      </c>
       <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>108</v>
+        <v>163</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F46" s="1">
-        <v>20000</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F47" s="9">
+        <v>10000</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>38</v>
@@ -3867,92 +3872,192 @@
         <v>45</v>
       </c>
       <c r="F50" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+      <c r="H50" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F53" s="1">
-        <v>30000</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="D58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3960,29 +4065,29 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AMK48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A34" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="31.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="1025" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4973,28 +5078,28 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AMK62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="33.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6287,30 +6392,30 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AMK44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7213,30 +7318,30 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:AMK10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7309,9 +7414,6 @@
       <c r="E5" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="F5" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -7329,9 +7431,6 @@
       <c r="E6" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="F6" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -7349,6 +7448,9 @@
       <c r="E7" s="18" t="s">
         <v>278</v>
       </c>
+      <c r="F7" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -7366,6 +7468,9 @@
       <c r="E8" s="18" t="s">
         <v>278</v>
       </c>
+      <c r="F8" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -7382,6 +7487,9 @@
       </c>
       <c r="E9" s="18" t="s">
         <v>278</v>
+      </c>
+      <c r="F9" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -7407,24 +7515,24 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A2:AMK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A2:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="1025" width="8.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -7444,7 +7552,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3 cases check in
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="294">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -2843,9 +2843,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -2867,9 +2865,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -2891,9 +2887,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -2913,9 +2907,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -2937,9 +2929,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -2959,9 +2949,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -2983,9 +2971,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -3005,9 +2991,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -3029,9 +3013,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -3051,9 +3033,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -3075,9 +3055,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -3099,9 +3077,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -3123,9 +3099,7 @@
         <v>68</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -3145,9 +3119,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -3169,9 +3141,7 @@
         <v>131</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -3193,9 +3163,7 @@
         <v>80</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -3215,9 +3183,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -3239,9 +3205,7 @@
         <v>3000</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -3261,9 +3225,7 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -3283,9 +3245,7 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -3305,9 +3265,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -3327,9 +3285,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -3349,9 +3305,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -3371,9 +3325,7 @@
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -3393,9 +3345,7 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -3415,9 +3365,7 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -3437,9 +3385,7 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -3461,9 +3407,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -3483,9 +3427,7 @@
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -3505,9 +3447,7 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -3529,9 +3469,7 @@
         <v>142</v>
       </c>
       <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -3553,9 +3491,7 @@
         <v>142</v>
       </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -3577,9 +3513,7 @@
         <v>43525</v>
       </c>
       <c r="G37" s="13"/>
-      <c r="H37" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -3601,9 +3535,7 @@
         <v>45743</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -3623,9 +3555,7 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -3645,9 +3575,7 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -3669,9 +3597,7 @@
         <v>155</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -3691,9 +3617,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -3715,9 +3639,7 @@
         <v>160</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -3737,9 +3659,7 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -3761,9 +3681,7 @@
         <v>5000</v>
       </c>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -3783,9 +3701,7 @@
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -3807,9 +3723,7 @@
         <v>10000</v>
       </c>
       <c r="G47" s="9"/>
-      <c r="H47" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -3829,9 +3743,7 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -3851,9 +3763,7 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -3875,9 +3785,7 @@
         <v>20000</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -3897,9 +3805,7 @@
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -3919,9 +3825,7 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -3941,9 +3845,7 @@
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -3965,9 +3867,7 @@
         <v>10000</v>
       </c>
       <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -3987,9 +3887,7 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -4009,9 +3907,7 @@
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
@@ -4033,9 +3929,7 @@
         <v>30000</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
@@ -4055,9 +3949,7 @@
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H58" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5180,7 +5072,9 @@
         <v>38</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -5202,7 +5096,9 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -5224,7 +5120,9 @@
         <v>182</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -5244,7 +5142,9 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -5266,7 +5166,9 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -5286,7 +5188,9 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -5308,7 +5212,9 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -5330,7 +5236,9 @@
         <v>2</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -5352,7 +5260,9 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -5372,7 +5282,9 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -5394,7 +5306,9 @@
         <v>64</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -5414,7 +5328,9 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -5434,7 +5350,9 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -5454,7 +5372,9 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -5474,7 +5394,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -5496,7 +5418,9 @@
         <v>168</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -5518,7 +5442,9 @@
         <v>193</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -5540,7 +5466,9 @@
         <v>68</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -5562,7 +5490,9 @@
         <v>5000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -5582,7 +5512,9 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -5604,7 +5536,9 @@
         <v>194</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -5626,7 +5560,9 @@
         <v>194</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -5646,7 +5582,9 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -5668,7 +5606,9 @@
         <v>3000</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -5688,7 +5628,9 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -5708,7 +5650,9 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -5728,7 +5672,9 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -5748,7 +5694,9 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -5770,7 +5718,9 @@
         <v>199</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -5790,7 +5740,9 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -5812,7 +5764,9 @@
         <v>199</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -5832,7 +5786,9 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -5854,7 +5810,9 @@
         <v>3000</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -5874,7 +5832,9 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -5894,7 +5854,9 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -5916,7 +5878,9 @@
         <v>204</v>
       </c>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -5938,7 +5902,9 @@
         <v>204</v>
       </c>
       <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="H41" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -5960,7 +5926,9 @@
         <v>43526</v>
       </c>
       <c r="G42" s="13"/>
-      <c r="H42" s="9"/>
+      <c r="H42" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -5982,7 +5950,9 @@
         <v>45743</v>
       </c>
       <c r="G43" s="13"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -6002,7 +5972,9 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -6022,7 +5994,9 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -6044,7 +6018,9 @@
         <v>155</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -6064,7 +6040,9 @@
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -6086,7 +6064,9 @@
         <v>207</v>
       </c>
       <c r="G48" s="1"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -6106,7 +6086,9 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -6128,7 +6110,9 @@
         <v>5000</v>
       </c>
       <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -6148,7 +6132,9 @@
       </c>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="H51" s="9" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -7448,9 +7434,6 @@
       <c r="E7" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="F7" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -7468,9 +7451,6 @@
       <c r="E8" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="F8" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -7487,9 +7467,6 @@
       </c>
       <c r="E9" s="18" t="s">
         <v>278</v>
-      </c>
-      <c r="F9" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:8">

</xml_diff>

<commit_message>
suite to run 3 scenarios
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{5E3BCD27-1CE0-45F8-AD5E-79BBC0639395}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{33BE9526-47DD-4644-9857-633FAB57CE37}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="4" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="294">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -554,9 +554,6 @@
     <t>hiddenClick</t>
   </si>
   <si>
-    <t>test_5</t>
-  </si>
-  <si>
     <t>select radio button</t>
   </si>
   <si>
@@ -909,6 +906,9 @@
   </si>
   <si>
     <t>uncheck cc</t>
+  </si>
+  <si>
+    <t>free_mobile</t>
   </si>
   <si>
     <t>Pass</t>
@@ -2369,10 +2369,10 @@
         <v>98</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>93</v>
@@ -2748,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView topLeftCell="A22" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3295,7 +3295,7 @@
         <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>95</v>
@@ -3358,7 +3358,7 @@
         <v>136</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>93</v>
@@ -3964,10 +3964,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4060,7 +4060,9 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -4082,7 +4084,9 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -4104,7 +4108,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -4124,7 +4130,9 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -4146,7 +4154,9 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -4166,7 +4176,9 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -4188,7 +4200,9 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -4208,7 +4222,9 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -4230,7 +4246,9 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -4250,7 +4268,9 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -4272,7 +4292,9 @@
         <v>168</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -4294,7 +4316,9 @@
         <v>64</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -4316,7 +4340,9 @@
         <v>68</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -4338,7 +4364,9 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -4358,7 +4386,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -4380,7 +4410,9 @@
         <v>169</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -4402,7 +4434,9 @@
         <v>80</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -4422,7 +4456,9 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -4444,7 +4480,9 @@
         <v>3000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -4464,7 +4502,9 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -4484,7 +4524,9 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -4504,120 +4546,126 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>38</v>
+        <v>91</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>288</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" s="1">
-        <v>3000</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="1">
-        <v>8000</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>170</v>
+        <v>82</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>173</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>44</v>
@@ -4629,69 +4677,77 @@
         <v>45</v>
       </c>
       <c r="F32" s="1">
-        <v>8000</v>
+        <v>3000</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>174</v>
+        <v>82</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>177</v>
+        <v>38</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F34" s="1">
+        <v>8000</v>
+      </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>170</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>171</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="1">
-        <v>3000</v>
+        <v>172</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>291</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -4701,55 +4757,59 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F36" s="1">
+        <v>8000</v>
+      </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>44</v>
+        <v>173</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>174</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="1">
-        <v>3000</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>49</v>
@@ -4763,18 +4823,20 @@
         <v>22</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>106</v>
+        <v>44</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3000</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
@@ -4783,20 +4845,18 @@
         <v>22</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F40" s="1">
-        <v>20000</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
@@ -4805,18 +4865,20 @@
         <v>22</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3000</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
@@ -4825,16 +4887,16 @@
         <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -4845,16 +4907,16 @@
         <v>22</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -4865,10 +4927,10 @@
         <v>22</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>38</v>
@@ -4877,7 +4939,7 @@
         <v>45</v>
       </c>
       <c r="F44" s="1">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -4887,16 +4949,16 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>165</v>
+        <v>124</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -4907,16 +4969,16 @@
         <v>22</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -4927,20 +4989,18 @@
         <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="1">
-        <v>30000</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
@@ -4949,20 +5009,104 @@
         <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F48" s="1">
+        <v>10000</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4977,10 +5121,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A34" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4996,7 +5140,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -5072,9 +5216,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -5096,9 +5238,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -5117,12 +5257,10 @@
         <v>45</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -5142,9 +5280,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -5166,9 +5302,7 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -5188,9 +5322,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -5212,9 +5344,7 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -5230,15 +5360,13 @@
         <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -5260,9 +5388,7 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -5272,19 +5398,17 @@
         <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -5294,7 +5418,7 @@
         <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>38</v>
@@ -5306,9 +5430,7 @@
         <v>64</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -5318,19 +5440,17 @@
         <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -5340,19 +5460,17 @@
         <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -5362,19 +5480,17 @@
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -5394,9 +5510,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -5418,9 +5532,7 @@
         <v>168</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -5439,12 +5551,10 @@
         <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -5466,9 +5576,7 @@
         <v>68</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -5490,9 +5598,7 @@
         <v>5000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -5512,9 +5618,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -5533,12 +5637,10 @@
         <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -5557,12 +5659,10 @@
         <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -5582,9 +5682,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -5606,9 +5704,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -5628,9 +5724,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -5650,9 +5744,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -5672,9 +5764,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -5684,19 +5774,17 @@
         <v>98</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>196</v>
+        <v>99</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -5706,21 +5794,17 @@
         <v>100</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>198</v>
+        <v>91</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>288</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -5730,19 +5814,17 @@
         <v>101</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>200</v>
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>198</v>
+        <v>95</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>201</v>
+        <v>93</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -5752,432 +5834,394 @@
         <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>202</v>
+        <v>91</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>82</v>
+        <v>194</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>44</v>
+        <v>196</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="1">
-        <v>3000</v>
+        <v>75</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>137</v>
+        <v>199</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>83</v>
+        <v>197</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>138</v>
+        <v>201</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>141</v>
+        <v>83</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F41" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F42" s="13">
-        <v>43526</v>
-      </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="13">
-        <v>45743</v>
-      </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>203</v>
+      </c>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F46" s="13">
+        <v>43526</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="F47" s="13">
+        <v>45743</v>
+      </c>
+      <c r="G47" s="13"/>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>206</v>
+        <v>149</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>153</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>208</v>
+        <v>156</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>83</v>
+        <v>204</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>209</v>
+        <v>158</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>199</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G52" s="1"/>
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E53" s="15" t="s">
+      <c r="B53" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
       <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8">
@@ -6188,15 +6232,17 @@
         <v>165</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>166</v>
+        <v>69</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>107</v>
+        <v>38</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F54" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F54" s="9">
+        <v>5000</v>
+      </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
     </row>
@@ -6205,21 +6251,19 @@
         <v>19</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>164</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>44</v>
+        <v>207</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="1">
-        <v>20000</v>
-      </c>
-      <c r="G55" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
       <c r="H55" s="9"/>
     </row>
     <row r="56" spans="1:8">
@@ -6227,41 +6271,43 @@
         <v>19</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>109</v>
+        <v>161</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>110</v>
+        <v>208</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+        <v>209</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>198</v>
+      </c>
       <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="1">
-        <v>60000</v>
-      </c>
-      <c r="G57" s="1"/>
+      <c r="B57" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
       <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8">
@@ -6269,19 +6315,19 @@
         <v>19</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8">
@@ -6289,7 +6335,7 @@
         <v>19</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>44</v>
@@ -6301,7 +6347,7 @@
         <v>45</v>
       </c>
       <c r="F59" s="1">
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="9"/>
@@ -6311,20 +6357,18 @@
         <v>19</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>211</v>
+        <v>110</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>212</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="9"/>
     </row>
@@ -6333,23 +6377,21 @@
         <v>19</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>213</v>
+        <v>120</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>214</v>
+        <v>45</v>
       </c>
       <c r="F61" s="1">
-        <v>123458</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>60000</v>
+      </c>
+      <c r="G61" s="1"/>
       <c r="H61" s="9"/>
     </row>
     <row r="62" spans="1:8">
@@ -6357,20 +6399,108 @@
         <v>19</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="9"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G63" s="1"/>
+      <c r="H63" s="9"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G64" s="1"/>
+      <c r="H64" s="9"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F65" s="1">
+        <v>123458</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H65" s="9"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6406,7 +6536,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -6523,7 +6653,7 @@
         <v>45</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="1"/>
@@ -6536,16 +6666,16 @@
         <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -6558,10 +6688,10 @@
         <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>49</v>
@@ -6578,10 +6708,10 @@
         <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>49</v>
@@ -6598,7 +6728,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>38</v>
@@ -6607,7 +6737,7 @@
         <v>63</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -6620,10 +6750,10 @@
         <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>49</v>
@@ -6640,10 +6770,10 @@
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>49</v>
@@ -6702,16 +6832,16 @@
         <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>229</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>230</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>154</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -6724,10 +6854,10 @@
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>233</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>49</v>
@@ -6753,7 +6883,7 @@
         <v>45</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -6766,13 +6896,13 @@
         <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F19" s="1">
         <v>3</v>
@@ -6788,13 +6918,13 @@
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -6808,13 +6938,13 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
@@ -6830,13 +6960,13 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -6850,13 +6980,13 @@
         <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
@@ -6872,10 +7002,10 @@
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>238</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>49</v>
@@ -6892,13 +7022,13 @@
         <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -6912,13 +7042,13 @@
         <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>243</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -6932,10 +7062,10 @@
         <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>49</v>
@@ -6952,13 +7082,13 @@
         <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -6974,13 +7104,13 @@
         <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>247</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -6994,7 +7124,7 @@
         <v>43</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>38</v>
@@ -7003,7 +7133,7 @@
         <v>63</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -7016,10 +7146,10 @@
         <v>43</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>49</v>
@@ -7036,13 +7166,13 @@
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -7056,7 +7186,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>38</v>
@@ -7065,7 +7195,7 @@
         <v>63</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -7078,10 +7208,10 @@
         <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>49</v>
@@ -7098,10 +7228,10 @@
         <v>43</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>49</v>
@@ -7118,7 +7248,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>38</v>
@@ -7140,13 +7270,13 @@
         <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -7160,7 +7290,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>38</v>
@@ -7182,7 +7312,7 @@
         <v>46</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>38</v>
@@ -7191,7 +7321,7 @@
         <v>63</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -7204,13 +7334,13 @@
         <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -7224,10 +7354,10 @@
         <v>46</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>49</v>
@@ -7244,13 +7374,13 @@
         <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -7264,7 +7394,7 @@
         <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>38</v>
@@ -7273,7 +7403,7 @@
         <v>63</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -7286,13 +7416,13 @@
         <v>50</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>269</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -7357,7 +7487,7 @@
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
@@ -7367,19 +7497,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>274</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -7389,16 +7519,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -7406,16 +7536,16 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>280</v>
-      </c>
       <c r="E6" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -7423,16 +7553,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>276</v>
-      </c>
       <c r="D7" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -7440,16 +7570,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C8" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -7457,16 +7587,16 @@
         <v>16</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>284</v>
-      </c>
       <c r="E9" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -7474,16 +7604,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D10" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>285</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -7517,7 +7647,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7525,7 +7655,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checking 4 scenarios to run
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{33BE9526-47DD-4644-9857-633FAB57CE37}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9EF3D7BE-6B62-4801-A961-8B0D6EBE203C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
     <workbookView activeTab="4" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1574" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="293">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -546,9 +546,6 @@
   </si>
   <si>
     <t>Delete the offer</t>
-  </si>
-  <si>
-    <t>rbdeloffer</t>
   </si>
   <si>
     <t>hiddenClick</t>
@@ -1856,7 +1853,7 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1880,7 +1877,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1904,7 +1901,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1926,7 +1923,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1950,7 +1947,7 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1972,7 +1969,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1996,7 +1993,7 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2018,7 +2015,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2042,7 +2039,7 @@
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2064,7 +2061,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2088,7 +2085,7 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2112,7 +2109,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2136,7 +2133,7 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2160,7 +2157,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2182,7 +2179,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2206,7 +2203,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2230,7 +2227,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2252,7 +2249,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2276,7 +2273,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2298,7 +2295,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2320,7 +2317,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2342,7 +2339,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2364,7 +2361,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2386,7 +2383,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2408,7 +2405,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2419,10 +2416,10 @@
         <v>98</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>93</v>
@@ -2430,7 +2427,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2452,7 +2449,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2476,7 +2473,7 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2498,7 +2495,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2522,7 +2519,7 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2544,7 +2541,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2568,7 +2565,7 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2590,7 +2587,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2612,7 +2609,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2636,7 +2633,7 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2658,7 +2655,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2680,7 +2677,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2702,7 +2699,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2726,7 +2723,7 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2748,7 +2745,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2770,7 +2767,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2794,7 +2791,7 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2816,7 +2813,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -2834,8 +2831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A49" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2930,7 +2927,7 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2954,7 +2951,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2978,7 +2975,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3000,7 +2997,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3024,7 +3021,7 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3046,7 +3043,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3070,7 +3067,7 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3092,7 +3089,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3116,7 +3113,7 @@
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3138,7 +3135,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3162,7 +3159,7 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3186,7 +3183,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -3210,7 +3207,7 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -3232,7 +3229,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -3256,7 +3253,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -3280,7 +3277,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3302,7 +3299,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3326,7 +3323,7 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3348,7 +3345,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3370,7 +3367,7 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -3392,7 +3389,7 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -3414,7 +3411,7 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -3425,7 +3422,7 @@
         <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>95</v>
@@ -3436,7 +3433,7 @@
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
       <c r="H27" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -3458,7 +3455,7 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
       <c r="H28" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -3480,7 +3477,7 @@
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
       <c r="H29" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -3494,7 +3491,7 @@
         <v>136</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>93</v>
@@ -3502,7 +3499,7 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -3524,7 +3521,7 @@
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
       <c r="H31" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -3548,7 +3545,7 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -3570,7 +3567,7 @@
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="H33" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -3592,7 +3589,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -3616,7 +3613,7 @@
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -3640,7 +3637,7 @@
       </c>
       <c r="G36" s="9"/>
       <c r="H36" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -3664,7 +3661,7 @@
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -3688,7 +3685,7 @@
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -3710,7 +3707,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
       <c r="H39" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -3732,7 +3729,7 @@
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -3756,7 +3753,7 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -3778,7 +3775,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -3802,7 +3799,7 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -3824,7 +3821,7 @@
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3848,7 +3845,7 @@
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3870,7 +3867,7 @@
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3894,7 +3891,7 @@
       </c>
       <c r="G47" s="9"/>
       <c r="H47" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3916,7 +3913,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3938,7 +3935,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3962,7 +3959,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3984,7 +3981,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -4006,7 +4003,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -4028,7 +4025,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -4052,7 +4049,7 @@
       </c>
       <c r="G54" s="1"/>
       <c r="H54" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -4074,7 +4071,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -4096,7 +4093,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -4120,7 +4117,7 @@
       </c>
       <c r="G57" s="1"/>
       <c r="H57" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -4142,7 +4139,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -4160,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4254,7 +4251,9 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -4276,7 +4275,9 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -4298,7 +4299,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -4318,7 +4321,9 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -4340,7 +4345,9 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -4360,7 +4367,9 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -4382,7 +4391,9 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -4402,7 +4413,9 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -4424,7 +4437,9 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -4444,7 +4459,9 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -4466,7 +4483,9 @@
         <v>168</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -4488,7 +4507,9 @@
         <v>64</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -4510,7 +4531,9 @@
         <v>68</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -4532,7 +4555,9 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -4552,7 +4577,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -4731,7 +4758,7 @@
         <v>91</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>93</v>
@@ -4875,13 +4902,13 @@
         <v>170</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>172</v>
-      </c>
       <c r="F35" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -4916,10 +4943,10 @@
         <v>102</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>49</v>
@@ -4936,10 +4963,10 @@
         <v>105</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>49</v>
@@ -5181,7 +5208,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>125</v>
@@ -5223,7 +5250,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>129</v>
@@ -5232,7 +5259,7 @@
         <v>38</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -5270,7 +5297,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -5347,7 +5374,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5371,7 +5398,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5391,11 +5418,11 @@
         <v>45</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5417,7 +5444,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5441,7 +5468,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5463,7 +5490,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5487,7 +5514,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5504,14 +5531,14 @@
         <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5535,7 +5562,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5546,10 +5573,10 @@
         <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>49</v>
@@ -5557,7 +5584,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -5568,7 +5595,7 @@
         <v>59</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>38</v>
@@ -5581,7 +5608,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -5592,10 +5619,10 @@
         <v>62</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>49</v>
@@ -5603,7 +5630,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -5614,10 +5641,10 @@
         <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>49</v>
@@ -5625,7 +5652,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -5636,18 +5663,18 @@
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -5669,7 +5696,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -5693,7 +5720,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -5713,11 +5740,11 @@
         <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -5741,7 +5768,7 @@
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -5765,7 +5792,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -5787,7 +5814,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -5807,11 +5834,11 @@
         <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -5831,11 +5858,11 @@
         <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -5857,7 +5884,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -5881,7 +5908,7 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -5903,7 +5930,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -5925,7 +5952,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -5947,7 +5974,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -5969,7 +5996,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -5983,7 +6010,7 @@
         <v>91</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>93</v>
@@ -5991,7 +6018,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -6013,7 +6040,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -6035,7 +6062,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -6046,10 +6073,10 @@
         <v>98</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>49</v>
@@ -6057,7 +6084,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -6068,20 +6095,20 @@
         <v>100</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -6092,18 +6119,18 @@
         <v>101</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -6114,20 +6141,20 @@
         <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -6149,7 +6176,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -6173,7 +6200,7 @@
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -6195,7 +6222,7 @@
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -6217,7 +6244,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -6237,11 +6264,11 @@
         <v>75</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -6261,11 +6288,11 @@
         <v>75</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G45" s="9"/>
       <c r="H45" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -6289,7 +6316,7 @@
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -6313,7 +6340,7 @@
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -6335,7 +6362,7 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -6357,7 +6384,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -6381,7 +6408,7 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -6395,7 +6422,7 @@
         <v>156</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>49</v>
@@ -6403,7 +6430,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -6417,17 +6444,17 @@
         <v>158</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>154</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -6449,7 +6476,7 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -6473,7 +6500,7 @@
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -6484,7 +6511,7 @@
         <v>164</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>83</v>
@@ -6495,7 +6522,7 @@
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -6506,22 +6533,22 @@
         <v>161</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="F56" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -6543,7 +6570,7 @@
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
       <c r="H57" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -6565,7 +6592,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -6589,7 +6616,7 @@
       </c>
       <c r="G59" s="1"/>
       <c r="H59" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -6611,7 +6638,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -6635,7 +6662,7 @@
       </c>
       <c r="G61" s="1"/>
       <c r="H61" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -6657,7 +6684,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -6681,7 +6708,7 @@
       </c>
       <c r="G63" s="1"/>
       <c r="H63" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -6692,7 +6719,7 @@
         <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>3</v>
@@ -6701,11 +6728,11 @@
         <v>4</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -6716,22 +6743,22 @@
         <v>127</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="F65" s="1">
         <v>123458</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H65" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -6753,7 +6780,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -6790,7 +6817,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -6907,7 +6934,7 @@
         <v>45</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="1"/>
@@ -6920,16 +6947,16 @@
         <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -6942,10 +6969,10 @@
         <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>49</v>
@@ -6962,10 +6989,10 @@
         <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>49</v>
@@ -6982,7 +7009,7 @@
         <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>38</v>
@@ -6991,7 +7018,7 @@
         <v>63</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -7004,10 +7031,10 @@
         <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>49</v>
@@ -7024,10 +7051,10 @@
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>49</v>
@@ -7086,16 +7113,16 @@
         <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>228</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>229</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>154</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -7108,10 +7135,10 @@
         <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>49</v>
@@ -7137,7 +7164,7 @@
         <v>45</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -7150,13 +7177,13 @@
         <v>43</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F19" s="1">
         <v>3</v>
@@ -7172,13 +7199,13 @@
         <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -7192,13 +7219,13 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F21" s="1">
         <v>2</v>
@@ -7214,13 +7241,13 @@
         <v>43</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
@@ -7234,13 +7261,13 @@
         <v>43</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F23" s="1">
         <v>1</v>
@@ -7256,10 +7283,10 @@
         <v>43</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>49</v>
@@ -7276,13 +7303,13 @@
         <v>43</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
@@ -7296,13 +7323,13 @@
         <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -7316,10 +7343,10 @@
         <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>49</v>
@@ -7336,13 +7363,13 @@
         <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F28" s="1">
         <v>2</v>
@@ -7358,13 +7385,13 @@
         <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -7378,7 +7405,7 @@
         <v>43</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>38</v>
@@ -7387,7 +7414,7 @@
         <v>63</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -7400,10 +7427,10 @@
         <v>43</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>49</v>
@@ -7420,13 +7447,13 @@
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -7440,7 +7467,7 @@
         <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>38</v>
@@ -7449,7 +7476,7 @@
         <v>63</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -7462,10 +7489,10 @@
         <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>49</v>
@@ -7482,10 +7509,10 @@
         <v>43</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>49</v>
@@ -7502,7 +7529,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>38</v>
@@ -7524,13 +7551,13 @@
         <v>43</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -7544,7 +7571,7 @@
         <v>43</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>38</v>
@@ -7566,7 +7593,7 @@
         <v>46</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>38</v>
@@ -7575,7 +7602,7 @@
         <v>63</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -7588,13 +7615,13 @@
         <v>43</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -7608,10 +7635,10 @@
         <v>46</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>49</v>
@@ -7628,13 +7655,13 @@
         <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -7648,7 +7675,7 @@
         <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>38</v>
@@ -7657,7 +7684,7 @@
         <v>63</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -7670,13 +7697,13 @@
         <v>50</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="E44" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -7741,7 +7768,7 @@
       <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G3" s="26"/>
       <c r="H3" s="26"/>
@@ -7751,19 +7778,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>270</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>271</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>273</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -7773,16 +7800,19 @@
         <v>0</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="D5" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>277</v>
+      <c r="F5" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -7790,16 +7820,19 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>279</v>
-      </c>
       <c r="E6" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="F6" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -7807,16 +7840,19 @@
         <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>275</v>
-      </c>
       <c r="D7" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="F7" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -7824,16 +7860,19 @@
         <v>16</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C8" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E8" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>277</v>
+      <c r="F8" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -7841,16 +7880,19 @@
         <v>16</v>
       </c>
       <c r="B9" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="D9" s="18" t="s">
         <v>282</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>283</v>
-      </c>
       <c r="E9" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="F9" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -7858,16 +7900,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D10" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>284</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -7901,7 +7943,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7909,7 +7951,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated the actionClass and testdata
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{9EF3D7BE-6B62-4801-A961-8B0D6EBE203C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{63C34059-38F0-43D4-B031-F407D3C6D4E3}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="5" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="293">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -881,12 +881,6 @@
     <t>offer_name</t>
   </si>
   <si>
-    <t>OfferRegr4819</t>
-  </si>
-  <si>
-    <t>ED_Offer_RenamedLabel_2</t>
-  </si>
-  <si>
     <t>Not Available</t>
   </si>
   <si>
@@ -908,10 +902,16 @@
     <t>free_mobile</t>
   </si>
   <si>
+    <t>radBtnTestFolder</t>
+  </si>
+  <si>
+    <t>Select TestFolder</t>
+  </si>
+  <si>
+    <t>free_mobile1</t>
+  </si>
+  <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1754,10 +1754,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A31" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1877,7 +1877,7 @@
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1923,7 +1923,7 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1969,7 +1969,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2015,7 +2015,7 @@
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="G13" s="9"/>
       <c r="H13" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2061,7 +2061,7 @@
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2133,7 +2133,7 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2179,7 +2179,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2249,7 +2249,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2295,7 +2295,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2317,7 +2317,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2339,7 +2339,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2361,7 +2361,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2383,7 +2383,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2405,7 +2405,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2416,10 +2416,10 @@
         <v>98</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>93</v>
@@ -2427,7 +2427,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2449,7 +2449,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2495,7 +2495,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2541,7 +2541,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2565,7 +2565,7 @@
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2587,7 +2587,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2609,7 +2609,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2632,75 +2632,67 @@
         <v>20000</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>112</v>
+        <v>44</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>116</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="11" t="s">
@@ -2710,111 +2702,121 @@
         <v>117</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="1">
-        <v>10000</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F44" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F44" s="1">
+        <v>10000</v>
+      </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F46" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2829,10 +2831,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A46" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2926,9 +2928,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -2950,9 +2950,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -2974,9 +2972,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -2996,9 +2992,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -3020,9 +3014,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -3042,9 +3034,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -3066,9 +3056,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -3088,9 +3076,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -3112,9 +3098,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -3134,9 +3118,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -3158,9 +3140,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -3182,9 +3162,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -3206,9 +3184,7 @@
         <v>68</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -3228,9 +3204,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -3252,9 +3226,7 @@
         <v>131</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -3276,9 +3248,7 @@
         <v>80</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -3298,9 +3268,7 @@
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -3322,9 +3290,7 @@
         <v>3000</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -3344,9 +3310,7 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -3366,9 +3330,7 @@
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -3388,9 +3350,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -3410,9 +3370,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -3422,7 +3380,7 @@
         <v>98</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>95</v>
@@ -3432,9 +3390,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -3454,9 +3410,7 @@
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -3476,9 +3430,7 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -3491,16 +3443,14 @@
         <v>136</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>93</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -3520,9 +3470,7 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -3544,9 +3492,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -3566,9 +3512,7 @@
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -3588,9 +3532,7 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -3612,9 +3554,7 @@
         <v>142</v>
       </c>
       <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -3636,9 +3576,7 @@
         <v>142</v>
       </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -3660,9 +3598,7 @@
         <v>43525</v>
       </c>
       <c r="G37" s="13"/>
-      <c r="H37" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -3684,9 +3620,7 @@
         <v>45743</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -3706,9 +3640,7 @@
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -3728,9 +3660,7 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -3752,9 +3682,7 @@
         <v>155</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -3774,9 +3702,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -3798,9 +3724,7 @@
         <v>160</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -3820,9 +3744,7 @@
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -3844,9 +3766,7 @@
         <v>5000</v>
       </c>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -3866,9 +3786,7 @@
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -3890,9 +3808,7 @@
         <v>10000</v>
       </c>
       <c r="G47" s="9"/>
-      <c r="H47" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -3912,9 +3828,7 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -3934,9 +3848,7 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -3958,75 +3870,67 @@
         <v>20000</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>112</v>
+        <v>290</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E53" s="12" t="s">
         <v>116</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -4036,111 +3940,121 @@
         <v>117</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F54" s="1">
-        <v>10000</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F55" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F55" s="1">
+        <v>10000</v>
+      </c>
       <c r="G55" s="1"/>
-      <c r="H55" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F57" s="1"/>
       <c r="G57" s="1"/>
-      <c r="H57" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D58" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="D59" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4155,10 +4069,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView topLeftCell="A31" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4251,9 +4165,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -4275,9 +4187,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -4299,9 +4209,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -4321,9 +4229,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -4345,9 +4251,7 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -4367,9 +4271,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -4391,9 +4293,7 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -4413,9 +4313,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -4437,9 +4335,7 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -4459,9 +4355,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -4483,9 +4377,7 @@
         <v>168</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -4507,9 +4399,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -4531,9 +4421,7 @@
         <v>68</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -4555,9 +4443,7 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -4577,9 +4463,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -4758,7 +4642,7 @@
         <v>91</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>93</v>
@@ -4908,7 +4792,7 @@
         <v>171</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -5106,16 +4990,16 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>112</v>
+        <v>44</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -5126,16 +5010,16 @@
         <v>22</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -5146,13 +5030,13 @@
         <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>116</v>
@@ -5166,20 +5050,18 @@
         <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="1">
-        <v>10000</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
@@ -5188,18 +5070,20 @@
         <v>22</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F49" s="1">
+        <v>10000</v>
+      </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
@@ -5208,16 +5092,16 @@
         <v>22</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -5228,20 +5112,18 @@
         <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
@@ -5250,20 +5132,42 @@
         <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F52" s="1">
+        <v>30000</v>
+      </c>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5278,10 +5182,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5373,9 +5277,7 @@
         <v>38</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -5397,9 +5299,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -5421,9 +5321,7 @@
         <v>180</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -5443,9 +5341,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -5467,9 +5363,7 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -5489,9 +5383,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -5513,9 +5405,7 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -5537,9 +5427,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -5561,9 +5449,7 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -5583,9 +5469,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -5607,9 +5491,7 @@
         <v>64</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -5629,9 +5511,7 @@
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -5651,9 +5531,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -5673,9 +5551,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -5695,9 +5571,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -5719,9 +5593,7 @@
         <v>168</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -5743,9 +5615,7 @@
         <v>191</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -5767,9 +5637,7 @@
         <v>68</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -5791,9 +5659,7 @@
         <v>5000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -5813,9 +5679,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -5837,9 +5701,7 @@
         <v>192</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -5861,9 +5723,7 @@
         <v>192</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -5883,9 +5743,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -5907,9 +5765,7 @@
         <v>3000</v>
       </c>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -5929,9 +5785,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -5951,9 +5805,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -5973,9 +5825,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -5995,9 +5845,7 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -6010,16 +5858,14 @@
         <v>91</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -6039,9 +5885,7 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -6061,9 +5905,7 @@
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -6083,9 +5925,7 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -6107,9 +5947,7 @@
         <v>197</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -6129,9 +5967,7 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -6153,9 +5989,7 @@
         <v>197</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -6175,9 +6009,7 @@
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -6199,9 +6031,7 @@
         <v>3000</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -6221,9 +6051,7 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -6243,9 +6071,7 @@
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -6267,9 +6093,7 @@
         <v>202</v>
       </c>
       <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -6291,9 +6115,7 @@
         <v>202</v>
       </c>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -6315,9 +6137,7 @@
         <v>43526</v>
       </c>
       <c r="G46" s="13"/>
-      <c r="H46" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -6339,9 +6159,7 @@
         <v>45743</v>
       </c>
       <c r="G47" s="13"/>
-      <c r="H47" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -6361,9 +6179,7 @@
       </c>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -6383,9 +6199,7 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -6407,9 +6221,7 @@
         <v>155</v>
       </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -6429,9 +6241,7 @@
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -6453,9 +6263,7 @@
         <v>205</v>
       </c>
       <c r="G52" s="1"/>
-      <c r="H52" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -6475,9 +6283,7 @@
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
-      <c r="H53" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H53" s="9"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -6499,9 +6305,7 @@
         <v>5000</v>
       </c>
       <c r="G54" s="9"/>
-      <c r="H54" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H54" s="9"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -6521,9 +6325,7 @@
       </c>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
-      <c r="H55" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H55" s="9"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -6547,9 +6349,7 @@
       <c r="G56" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="H56" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H56" s="9"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
@@ -6569,9 +6369,7 @@
       </c>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
-      <c r="H57" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
@@ -6591,9 +6389,7 @@
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
-      <c r="H58" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
@@ -6615,101 +6411,89 @@
         <v>20000</v>
       </c>
       <c r="G59" s="1"/>
-      <c r="H59" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H59" s="9"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>112</v>
+        <v>44</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
-      <c r="H60" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F61" s="1">
-        <v>60000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H61" s="9"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F62" s="1">
+        <v>60000</v>
+      </c>
       <c r="G62" s="1"/>
-      <c r="H62" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H62" s="9"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F63" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1"/>
-      <c r="H63" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H63" s="9"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
@@ -6719,21 +6503,19 @@
         <v>127</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>209</v>
+        <v>44</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>210</v>
+        <v>45</v>
+      </c>
+      <c r="F64" s="1">
+        <v>30000</v>
       </c>
       <c r="G64" s="1"/>
-      <c r="H64" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H64" s="9"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
@@ -6743,45 +6525,63 @@
         <v>127</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F65" s="1">
-        <v>123458</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="H65" s="9" t="s">
-        <v>292</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G65" s="1"/>
+      <c r="H65" s="9"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F66" s="1">
+        <v>123458</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H66" s="9"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E66" s="1" t="s">
+      <c r="D67" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6798,8 +6598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A34" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7722,10 +7522,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7811,9 +7611,6 @@
       <c r="E5" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F5" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -7831,9 +7628,6 @@
       <c r="E6" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F6" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -7851,9 +7645,6 @@
       <c r="E7" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F7" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -7871,9 +7662,6 @@
       <c r="E8" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F8" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -7886,13 +7674,10 @@
         <v>281</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>282</v>
+        <v>142</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>276</v>
-      </c>
-      <c r="F9" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -7906,10 +7691,27 @@
         <v>281</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>284</v>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -7943,7 +7745,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7951,7 +7753,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First check in on 51619
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{E719EFB7-82EC-4159-8DFF-E9C735E82A3B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7CF96C99-6828-4E73-8325-25C8E74BF65C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
     <workbookView activeTab="5" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1501" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="294">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1123,6 +1123,9 @@
     <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -1141,9 +1144,6 @@
     <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1632,22 +1632,22 @@
   </cols>
   <sheetData>
     <row customFormat="1" ht="14.25" r="1" s="3" spans="1:5">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row customFormat="1" ht="14.25" r="2" s="3" spans="1:5">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row customFormat="1" ht="14.25" r="3" s="3" spans="1:5">
       <c r="A3" s="4"/>
@@ -1760,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="A34" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="A41" sqref="A41:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1779,38 +1779,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
@@ -2597,18 +2597,20 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>111</v>
+        <v>44</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F41" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F41" s="1">
+        <v>7000</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
@@ -2617,16 +2619,16 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -2637,13 +2639,13 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E43" s="12" t="s">
         <v>116</v>
@@ -2660,17 +2662,15 @@
         <v>117</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="1">
-        <v>10000</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
@@ -2679,18 +2679,20 @@
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F45" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F45" s="1">
+        <v>10000</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
@@ -2699,16 +2701,16 @@
         <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2719,20 +2721,18 @@
         <v>0</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
@@ -2741,20 +2741,42 @@
         <v>0</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F48" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F48" s="1">
+        <v>30000</v>
+      </c>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2769,10 +2791,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A46" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D53" sqref="D53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2787,38 +2809,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -2866,7 +2888,9 @@
         <v>38</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -2888,7 +2912,9 @@
         <v>38</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -2910,7 +2936,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -2930,7 +2958,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -2952,7 +2982,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -2972,7 +3004,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -2994,7 +3028,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -3014,7 +3050,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -3036,7 +3074,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -3056,7 +3096,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -3078,7 +3120,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -3100,7 +3144,9 @@
         <v>64</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -3122,7 +3168,9 @@
         <v>68</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -3144,7 +3192,9 @@
         <v>7000</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -3164,7 +3214,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -3186,7 +3238,9 @@
         <v>131</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -3208,7 +3262,9 @@
         <v>80</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="9"/>
+      <c r="H21" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -3228,7 +3284,9 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -3250,7 +3308,9 @@
         <v>3000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -3270,7 +3330,9 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="9"/>
+      <c r="H24" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -3290,7 +3352,9 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -3310,7 +3374,9 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -3330,7 +3396,9 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -3350,7 +3418,9 @@
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="H28" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -3370,7 +3440,9 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -3390,7 +3462,9 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -3410,7 +3484,9 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -3430,7 +3506,9 @@
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="H32" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -3452,7 +3530,9 @@
         <v>3000</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -3472,7 +3552,9 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -3492,7 +3574,9 @@
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="H35" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -3514,7 +3598,9 @@
         <v>142</v>
       </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="H36" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -3536,7 +3622,9 @@
         <v>142</v>
       </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -3558,7 +3646,9 @@
         <v>43525</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -3580,7 +3670,9 @@
         <v>45743</v>
       </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -3600,7 +3692,9 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -3620,7 +3714,9 @@
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="H41" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -3642,7 +3738,9 @@
         <v>155</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="9"/>
+      <c r="H42" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -3662,7 +3760,9 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -3684,7 +3784,9 @@
         <v>160</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -3704,7 +3806,9 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -3726,7 +3830,9 @@
         <v>5000</v>
       </c>
       <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -3746,7 +3852,9 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -3768,7 +3876,9 @@
         <v>10000</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -3788,7 +3898,9 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -3808,7 +3920,9 @@
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -3830,7 +3944,9 @@
         <v>20000</v>
       </c>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
+      <c r="H51" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -3850,67 +3966,77 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
+      <c r="H52" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>111</v>
+        <v>290</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F53" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F53" s="1">
+        <v>7000</v>
+      </c>
       <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
+      <c r="H53" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
+      <c r="H54" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>116</v>
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="H55" s="1" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -3920,101 +4046,133 @@
         <v>117</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="1">
-        <v>10000</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F57" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F57" s="1">
+        <v>10000</v>
+      </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+      <c r="H57" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+      <c r="H58" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F59" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="D61" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1" t="s">
+        <v>292</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4029,10 +4187,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A34" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="D46" sqref="D46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4048,38 +4206,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -4125,9 +4283,7 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -4149,9 +4305,7 @@
         <v>38</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -4173,9 +4327,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -4195,9 +4347,7 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -4219,9 +4369,7 @@
         <v>167</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -4241,9 +4389,7 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -4265,9 +4411,7 @@
         <v>168</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -4287,9 +4431,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -4311,9 +4453,7 @@
         <v>168</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -4333,9 +4473,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -4357,9 +4495,7 @@
         <v>168</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -4381,9 +4517,7 @@
         <v>64</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -4405,9 +4539,7 @@
         <v>68</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -4429,9 +4561,7 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -4451,9 +4581,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -4475,9 +4603,7 @@
         <v>169</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -4499,9 +4625,7 @@
         <v>80</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -4521,9 +4645,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -4545,9 +4667,7 @@
         <v>3000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -4567,9 +4687,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -4589,9 +4707,7 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -4611,9 +4727,7 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -4633,9 +4747,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -4655,9 +4767,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -4677,9 +4787,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -4699,9 +4807,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -4721,9 +4827,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -4745,9 +4849,7 @@
         <v>3000</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -4767,9 +4869,7 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -4791,9 +4891,7 @@
         <v>8000</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -4815,9 +4913,7 @@
         <v>288</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -4839,9 +4935,7 @@
         <v>8000</v>
       </c>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -4861,9 +4955,7 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -4883,9 +4975,7 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -4907,9 +4997,7 @@
         <v>3000</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -4929,9 +5017,7 @@
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -4953,9 +5039,7 @@
         <v>3000</v>
       </c>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -4975,9 +5059,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -4997,9 +5079,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -5021,9 +5101,7 @@
         <v>20000</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -5043,189 +5121,193 @@
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>293</v>
-      </c>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>111</v>
+        <v>44</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F46" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F46" s="1">
+        <v>7000</v>
+      </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>116</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
-      <c r="H48" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F49" s="1">
-        <v>10000</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
-      <c r="H49" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F50" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F50" s="1">
+        <v>10000</v>
+      </c>
       <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F52" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E53" s="1" t="s">
+      <c r="D54" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5240,10 +5322,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="A57" sqref="A57:D57"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5258,36 +5340,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -6422,13 +6504,13 @@
       <c r="D57" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E57" s="28" t="s">
+      <c r="E57" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F57" s="29">
+      <c r="F57" s="23">
         <v>5000</v>
       </c>
-      <c r="G57" s="27"/>
+      <c r="G57" s="21"/>
       <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8">
@@ -6518,18 +6600,20 @@
         <v>19</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>111</v>
+        <v>44</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F62" s="1">
+        <v>7000</v>
+      </c>
       <c r="G62" s="1"/>
       <c r="H62" s="9"/>
     </row>
@@ -6538,20 +6622,18 @@
         <v>19</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F63" s="1">
-        <v>60000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="9"/>
     </row>
@@ -6560,18 +6642,20 @@
         <v>19</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F64" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F64" s="1">
+        <v>60000</v>
+      </c>
       <c r="G64" s="1"/>
       <c r="H64" s="9"/>
     </row>
@@ -6580,20 +6664,18 @@
         <v>19</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F65" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="9"/>
     </row>
@@ -6605,16 +6687,16 @@
         <v>127</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>209</v>
+        <v>44</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>210</v>
+        <v>45</v>
+      </c>
+      <c r="F66" s="1">
+        <v>30000</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66" s="9"/>
@@ -6627,20 +6709,18 @@
         <v>127</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="F67" s="1">
-        <v>123458</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>197</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G67" s="1"/>
       <c r="H67" s="9"/>
     </row>
     <row r="68" spans="1:8">
@@ -6648,20 +6728,44 @@
         <v>19</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="F68" s="1">
+        <v>123458</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H68" s="9"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E68" s="1" t="s">
+      <c r="D69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="9"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6696,36 +6800,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -7622,36 +7726,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29" t="s">
         <v>268</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -7725,6 +7829,9 @@
       <c r="E7" s="18" t="s">
         <v>276</v>
       </c>
+      <c r="F7" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -7742,6 +7849,9 @@
       <c r="E8" s="18" t="s">
         <v>276</v>
       </c>
+      <c r="F8" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -7759,6 +7869,9 @@
       <c r="E9" s="18" t="s">
         <v>276</v>
       </c>
+      <c r="F9" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -7776,9 +7889,6 @@
       <c r="E10" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="F10" t="s">
-        <v>293</v>
-      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -7795,9 +7905,6 @@
       </c>
       <c r="E11" s="18" t="s">
         <v>282</v>
-      </c>
-      <c r="F11" t="s">
-        <v>292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit on 5/21/19 added few options in the openURL
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="291">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1574,7 +1574,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1614,12 +1614,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="2" width="14.5703125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" style="2" width="27.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" style="2" width="70.7109375" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" style="2" width="19.140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" style="2" width="24.42578125" collapsed="false"/>
-    <col min="6" max="1025" customWidth="true" style="2" width="9.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="70.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="24.42578125" collapsed="true"/>
+    <col min="6" max="1025" customWidth="true" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" ht="14.25" r="1" s="3" spans="1:5">
@@ -1759,14 +1759,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="39.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="false"/>
-    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="false"/>
-    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1873,7 +1873,9 @@
         <v>37</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -1895,7 +1897,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -1915,7 +1919,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -1937,7 +1943,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -1957,7 +1965,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -1979,7 +1989,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -1999,7 +2011,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -2021,7 +2035,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -2792,13 +2808,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="8.5703125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="34.85546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="30.85546875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="26.5703125" collapsed="false"/>
-    <col min="7" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="7" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4074,14 +4090,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="39.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="false"/>
-    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="false"/>
-    <col min="9" max="1025" customWidth="true" width="9.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -5209,13 +5225,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="28.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="33.140625" collapsed="false"/>
-    <col min="6" max="7" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="8" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6645,15 +6661,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="35.85546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="38.7109375" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="24.42578125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="21.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="8.140625" collapsed="false"/>
-    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7533,15 +7549,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="28.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="15.28515625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="18.0" collapsed="false"/>
-    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7738,9 +7754,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.5703125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="false"/>
-    <col min="3" max="1025" customWidth="true" width="8.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">

</xml_diff>

<commit_message>
check in to run 4 scenarios
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{204B1757-A26F-43DF-9CE7-3C4AB55A345B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{0F793908-24F3-49D3-B2CC-953F1F59BCE5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="5" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="6" firstSheet="5" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="292">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -909,9 +909,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -2893,9 +2890,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -2917,9 +2912,7 @@
         <v>37</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -2941,9 +2934,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -2963,9 +2954,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -2987,9 +2976,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -3009,9 +2996,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -3033,9 +3018,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -3055,9 +3038,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -3079,9 +3060,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -3101,9 +3080,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -3125,9 +3102,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -3149,9 +3124,7 @@
         <v>63</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -3173,9 +3146,7 @@
         <v>67</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -3197,9 +3168,7 @@
         <v>7000</v>
       </c>
       <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -3219,9 +3188,7 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -3243,9 +3210,7 @@
         <v>130</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -3267,9 +3232,7 @@
         <v>79</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -3289,9 +3252,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -3313,9 +3274,7 @@
         <v>3000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -3335,9 +3294,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -3357,9 +3314,7 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -3379,9 +3334,7 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -3401,9 +3354,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -3423,9 +3374,7 @@
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -3445,9 +3394,7 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -3467,9 +3414,7 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -3489,9 +3434,7 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -3511,9 +3454,7 @@
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -3535,9 +3476,7 @@
         <v>3000</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -3557,9 +3496,7 @@
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -3579,9 +3516,7 @@
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -3603,9 +3538,7 @@
         <v>141</v>
       </c>
       <c r="G36" s="9"/>
-      <c r="H36" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -3627,9 +3560,7 @@
         <v>141</v>
       </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -3651,9 +3582,7 @@
         <v>43525</v>
       </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -3675,9 +3604,7 @@
         <v>45743</v>
       </c>
       <c r="G39" s="13"/>
-      <c r="H39" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -3697,9 +3624,7 @@
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H40" s="9"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -3719,9 +3644,7 @@
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -3743,9 +3666,7 @@
         <v>154</v>
       </c>
       <c r="G42" s="1"/>
-      <c r="H42" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -3765,9 +3686,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H43" s="9"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -3789,9 +3708,7 @@
         <v>159</v>
       </c>
       <c r="G44" s="1"/>
-      <c r="H44" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -3811,9 +3728,7 @@
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H45" s="9"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -3835,9 +3750,7 @@
         <v>5000</v>
       </c>
       <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -3857,9 +3770,7 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -3881,9 +3792,7 @@
         <v>10000</v>
       </c>
       <c r="G48" s="9"/>
-      <c r="H48" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H48" s="9"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -3903,9 +3812,7 @@
       </c>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H49" s="9"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -3925,9 +3832,7 @@
       </c>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
-      <c r="H50" s="9" t="s">
-        <v>291</v>
-      </c>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -3949,9 +3854,7 @@
         <v>20000</v>
       </c>
       <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -3971,9 +3874,7 @@
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -3995,9 +3896,7 @@
         <v>7000</v>
       </c>
       <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -4017,9 +3916,7 @@
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -4039,9 +3936,7 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -4061,9 +3956,7 @@
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
-      <c r="H56" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
@@ -4085,9 +3978,7 @@
         <v>10000</v>
       </c>
       <c r="G57" s="1"/>
-      <c r="H57" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
@@ -4107,9 +3998,7 @@
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
-      <c r="H58" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
@@ -4129,9 +4018,7 @@
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
-      <c r="H59" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
@@ -4153,9 +4040,7 @@
         <v>30000</v>
       </c>
       <c r="G60" s="1"/>
-      <c r="H60" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
@@ -4175,9 +4060,7 @@
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
-      <c r="H61" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H61" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6765,8 +6648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7734,9 +7617,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -7756,9 +7637,7 @@
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -7780,9 +7659,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -7802,9 +7679,7 @@
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="9" t="s">
-        <v>292</v>
-      </c>
+      <c r="H46" s="9"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -7824,9 +7699,7 @@
       </c>
       <c r="F47" s="25"/>
       <c r="G47" s="25"/>
-      <c r="H47" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="H47" s="25"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -7848,9 +7721,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="25"/>
-      <c r="H48" s="25" t="s">
-        <v>291</v>
-      </c>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -7870,9 +7741,7 @@
       </c>
       <c r="F49" s="25"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="25" t="s">
-        <v>292</v>
-      </c>
+      <c r="H49" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7890,7 +7759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -8011,9 +7880,6 @@
       <c r="E7" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="F7" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -8031,9 +7897,6 @@
       <c r="E8" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="F8" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -8050,9 +7913,6 @@
       </c>
       <c r="E9" s="18" t="s">
         <v>272</v>
-      </c>
-      <c r="F9" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:8">

</xml_diff>

<commit_message>
added realitime spine script
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B1777103-F85A-4194-AA16-E50823627D69}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{B9D4E062-E4C1-4A75-BA6C-3E2D08B76BDF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="4" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="6" firstSheet="5" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="329">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -972,6 +972,51 @@
   </si>
   <si>
     <t xml:space="preserve">toggle </t>
+  </si>
+  <si>
+    <t>switching to parent frame</t>
+  </si>
+  <si>
+    <t>btnEngineConfigFilter</t>
+  </si>
+  <si>
+    <t>filter click</t>
+  </si>
+  <si>
+    <t>txtSearchbox</t>
+  </si>
+  <si>
+    <t>btnApply</t>
+  </si>
+  <si>
+    <t>LoadType</t>
+  </si>
+  <si>
+    <t>enter the loadtype</t>
+  </si>
+  <si>
+    <t>clcik apply</t>
+  </si>
+  <si>
+    <t>verifyLoadType</t>
+  </si>
+  <si>
+    <t>ensure loadtype is delta</t>
+  </si>
+  <si>
+    <t>txtValue</t>
+  </si>
+  <si>
+    <t>toggle button click</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>realtimeSpineAPIPostRequest</t>
+  </si>
+  <si>
+    <t>post api request to insert in to spine</t>
   </si>
   <si>
     <t>Pass</t>
@@ -984,7 +1029,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1029,6 +1074,12 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -1161,9 +1212,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
@@ -1214,9 +1266,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{58C6B9B9-44EF-4FF6-B4E2-0E7E1176543B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
@@ -4145,7 +4198,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="D10" sqref="D10:F16"/>
+      <selection activeCell="C8" sqref="C8:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5279,8 +5332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D10" sqref="D10:F15"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="C15" sqref="C15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6713,10 +6766,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6811,7 +6864,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -6835,7 +6888,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -6859,7 +6912,7 @@
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -6883,7 +6936,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -6907,7 +6960,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -6931,7 +6984,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -6955,7 +7008,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -6977,7 +7030,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -6999,7 +7052,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -7021,7 +7074,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -7045,7 +7098,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -7069,7 +7122,7 @@
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -7091,7 +7144,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -7115,7 +7168,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -7139,7 +7192,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -7161,7 +7214,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -7185,7 +7238,7 @@
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -7207,7 +7260,7 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -7231,7 +7284,7 @@
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -7255,7 +7308,7 @@
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -7277,7 +7330,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -7299,7 +7352,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -7321,7 +7374,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -7343,7 +7396,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -7367,7 +7420,7 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -7389,7 +7442,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -7413,7 +7466,7 @@
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -7435,7 +7488,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -7457,7 +7510,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -7481,7 +7534,7 @@
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -7503,7 +7556,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -7525,7 +7578,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -7549,7 +7602,7 @@
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -7571,7 +7624,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -7595,7 +7648,7 @@
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -7619,7 +7672,7 @@
       </c>
       <c r="G40" s="1"/>
       <c r="H40" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -7641,7 +7694,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -7663,7 +7716,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -7687,7 +7740,7 @@
       </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -7709,7 +7762,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -7731,7 +7784,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -7755,7 +7808,7 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -7777,7 +7830,7 @@
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -7799,7 +7852,7 @@
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
       <c r="H48" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -7823,7 +7876,7 @@
       </c>
       <c r="G49" s="25"/>
       <c r="H49" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -7845,7 +7898,7 @@
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
       <c r="H50" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -7867,7 +7920,7 @@
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -7891,7 +7944,7 @@
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -7913,7 +7966,7 @@
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
       <c r="H53" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -7935,7 +7988,7 @@
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -7957,7 +8010,7 @@
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
       <c r="H55" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -7979,7 +8032,7 @@
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -8001,7 +8054,7 @@
       <c r="F57" s="25"/>
       <c r="G57" s="25"/>
       <c r="H57" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -8025,7 +8078,7 @@
       </c>
       <c r="G58" s="25"/>
       <c r="H58" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -8049,7 +8102,7 @@
       </c>
       <c r="G59" s="25"/>
       <c r="H59" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -8073,7 +8126,7 @@
       </c>
       <c r="G60" s="25"/>
       <c r="H60" s="25" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -8081,190 +8134,462 @@
         <v>25</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="E61" s="26" t="s">
-        <v>302</v>
-      </c>
-      <c r="F61" s="26" t="s">
-        <v>307</v>
-      </c>
+      <c r="E61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F61" s="26"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+      <c r="H61" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>308</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F62" s="1"/>
+        <v>303</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="F62" s="26" t="s">
+        <v>307</v>
+      </c>
       <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
+      <c r="H62" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>167</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
+      <c r="H63" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C64" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="F64" s="1">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
+      <c r="H64" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>298</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>167</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
+      <c r="H65" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C66" s="26" t="s">
-        <v>310</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>182</v>
+        <v>309</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F66" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G66" s="25"/>
-      <c r="H66" s="25"/>
+      <c r="H66" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="D67" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>63</v>
+        <v>180</v>
+      </c>
+      <c r="F67" s="1">
+        <v>2</v>
       </c>
       <c r="G67" s="25"/>
-      <c r="H67" s="25"/>
+      <c r="H67" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C68" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="D68" s="26" t="s">
-        <v>304</v>
-      </c>
-      <c r="E68" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="F68" s="25"/>
+        <v>310</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
+      <c r="H68" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F69" s="1"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G71" s="25"/>
+      <c r="H71" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C72" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="E72" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="F72" s="25"/>
+      <c r="G72" s="25"/>
+      <c r="H72" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G73" s="25"/>
+      <c r="H73" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C74" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="D69" s="26" t="s">
+      <c r="D74" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="E69" s="26" t="s">
+      <c r="E74" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="D75" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="E75" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" s="25"/>
+      <c r="G75" s="25"/>
+      <c r="H75" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="D76" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E76" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" s="25">
+        <v>5000</v>
+      </c>
+      <c r="G76" s="25"/>
+      <c r="H76" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="D77" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E77" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F77" s="25" t="s">
+        <v>318</v>
+      </c>
+      <c r="G77" s="25"/>
+      <c r="H77" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C78" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="D78" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="E78" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F78" s="25"/>
+      <c r="G78" s="25"/>
+      <c r="H78" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C79" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="E79" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="F79" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="G79" s="25"/>
+      <c r="H79" s="25" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E80" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="25" t="s">
+        <v>328</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8488,7 +8813,7 @@
   <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
run for all 5 cases ..529
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{B9D4E062-E4C1-4A75-BA6C-3E2D08B76BDF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{077B0738-AED3-4F96-9DAC-E2D270F22B14}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="5" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="2" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="330">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1020,6 +1020,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1980,7 +1983,9 @@
         <v>37</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -2002,7 +2007,9 @@
         <v>37</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -2024,7 +2031,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -2044,7 +2053,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -2066,7 +2077,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -2086,7 +2099,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -2108,7 +2123,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -2128,7 +2145,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -2150,7 +2169,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -2170,7 +2191,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -2192,7 +2215,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -2214,7 +2239,9 @@
         <v>63</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -2236,7 +2263,9 @@
         <v>67</v>
       </c>
       <c r="G17" s="9"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="11" t="s">
@@ -2258,7 +2287,9 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
@@ -2278,7 +2309,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="11" t="s">
@@ -2300,7 +2333,9 @@
         <v>75</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="11" t="s">
@@ -2322,7 +2357,9 @@
         <v>79</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="11" t="s">
@@ -2342,7 +2379,9 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="11" t="s">
@@ -2364,7 +2403,9 @@
         <v>3000</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="11" t="s">
@@ -6768,8 +6809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E80" sqref="E80"/>
+    <sheetView topLeftCell="A70" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6863,9 +6904,7 @@
         <v>37</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -6887,9 +6926,7 @@
         <v>37</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -6911,9 +6948,7 @@
         <v>179</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -6935,9 +6970,7 @@
         <v>215</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -6959,9 +6992,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -6983,9 +7014,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -7007,9 +7036,7 @@
         <v>221</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -7029,9 +7056,7 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -7051,9 +7076,7 @@
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -7073,9 +7096,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -7097,9 +7118,7 @@
         <v>167</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -7121,9 +7140,7 @@
         <v>228</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -7143,9 +7160,7 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -7167,9 +7182,7 @@
         <v>179</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -7191,9 +7204,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -7213,9 +7224,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -7237,9 +7246,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -7259,9 +7266,7 @@
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -7283,9 +7288,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -7307,9 +7310,7 @@
         <v>215</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -7329,9 +7330,7 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -7351,9 +7350,7 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -7373,9 +7370,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -7395,9 +7390,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -7419,9 +7412,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -7441,9 +7432,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -7465,9 +7454,7 @@
         <v>245</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -7487,9 +7474,7 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -7509,9 +7494,7 @@
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -7533,9 +7516,7 @@
         <v>250</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -7555,9 +7536,7 @@
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -7577,9 +7556,7 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -7601,9 +7578,7 @@
         <v>3000</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -7623,9 +7598,7 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -7647,9 +7620,7 @@
         <v>2</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -7671,9 +7642,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -7693,9 +7662,7 @@
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -7715,9 +7682,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -7739,9 +7704,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -7761,9 +7724,7 @@
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -7783,9 +7744,7 @@
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
-      <c r="H45" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -7807,9 +7766,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="1"/>
-      <c r="H46" s="1" t="s">
-        <v>328</v>
-      </c>
+      <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -7829,9 +7786,7 @@
       </c>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="9" t="s">
-        <v>328</v>
-      </c>
+      <c r="H47" s="9"/>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -7851,9 +7806,7 @@
       </c>
       <c r="F48" s="25"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -7875,9 +7828,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="25"/>
-      <c r="H49" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H49" s="25"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -7897,9 +7848,7 @@
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
-      <c r="H50" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H50" s="25"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -7919,9 +7868,7 @@
       </c>
       <c r="F51" s="25"/>
       <c r="G51" s="25"/>
-      <c r="H51" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H51" s="25"/>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -7943,9 +7890,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="25"/>
-      <c r="H52" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H52" s="25"/>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -7965,9 +7910,7 @@
       </c>
       <c r="F53" s="25"/>
       <c r="G53" s="25"/>
-      <c r="H53" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H53" s="25"/>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -7987,9 +7930,7 @@
       </c>
       <c r="F54" s="25"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H54" s="25"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -8009,9 +7950,7 @@
       </c>
       <c r="F55" s="25"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H55" s="25"/>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -8031,9 +7970,7 @@
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="25"/>
-      <c r="H56" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H56" s="25"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
@@ -8053,9 +7990,7 @@
       </c>
       <c r="F57" s="25"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H57" s="25"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
@@ -8077,9 +8012,7 @@
         <v>8000</v>
       </c>
       <c r="G58" s="25"/>
-      <c r="H58" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H58" s="25"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
@@ -8101,9 +8034,7 @@
         <v>221</v>
       </c>
       <c r="G59" s="25"/>
-      <c r="H59" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H59" s="25"/>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
@@ -8125,9 +8056,7 @@
         <v>301</v>
       </c>
       <c r="G60" s="25"/>
-      <c r="H60" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H60" s="25"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
@@ -8147,9 +8076,7 @@
       </c>
       <c r="F61" s="26"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H61" s="25"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
@@ -8171,9 +8098,7 @@
         <v>307</v>
       </c>
       <c r="G62" s="25"/>
-      <c r="H62" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H62" s="25"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
@@ -8193,9 +8118,7 @@
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="25"/>
-      <c r="H63" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H63" s="25"/>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
@@ -8217,9 +8140,7 @@
         <v>166</v>
       </c>
       <c r="G64" s="25"/>
-      <c r="H64" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H64" s="25"/>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
@@ -8239,9 +8160,7 @@
       </c>
       <c r="F65" s="1"/>
       <c r="G65" s="25"/>
-      <c r="H65" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H65" s="25"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
@@ -8263,9 +8182,7 @@
         <v>167</v>
       </c>
       <c r="G66" s="25"/>
-      <c r="H66" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H66" s="25"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
@@ -8287,9 +8204,7 @@
         <v>2</v>
       </c>
       <c r="G67" s="25"/>
-      <c r="H67" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H67" s="25"/>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
@@ -8311,9 +8226,7 @@
         <v>167</v>
       </c>
       <c r="G68" s="25"/>
-      <c r="H68" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H68" s="25"/>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
@@ -8333,9 +8246,7 @@
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="25"/>
-      <c r="H69" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H69" s="25"/>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
@@ -8357,9 +8268,7 @@
         <v>63</v>
       </c>
       <c r="G70" s="25"/>
-      <c r="H70" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H70" s="25"/>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
@@ -8381,9 +8290,7 @@
         <v>5000</v>
       </c>
       <c r="G71" s="25"/>
-      <c r="H71" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H71" s="25"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
@@ -8403,9 +8310,7 @@
       </c>
       <c r="F72" s="25"/>
       <c r="G72" s="25"/>
-      <c r="H72" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H72" s="25"/>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
@@ -8427,9 +8332,7 @@
         <v>2000</v>
       </c>
       <c r="G73" s="25"/>
-      <c r="H73" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H73" s="25"/>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
@@ -8449,9 +8352,7 @@
       </c>
       <c r="F74" s="25"/>
       <c r="G74" s="25"/>
-      <c r="H74" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H74" s="25"/>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
@@ -8471,9 +8372,7 @@
       </c>
       <c r="F75" s="25"/>
       <c r="G75" s="25"/>
-      <c r="H75" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H75" s="25"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
@@ -8495,9 +8394,7 @@
         <v>5000</v>
       </c>
       <c r="G76" s="25"/>
-      <c r="H76" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H76" s="25"/>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
@@ -8519,9 +8416,7 @@
         <v>318</v>
       </c>
       <c r="G77" s="25"/>
-      <c r="H77" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H77" s="25"/>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
@@ -8541,9 +8436,7 @@
       </c>
       <c r="F78" s="25"/>
       <c r="G78" s="25"/>
-      <c r="H78" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
@@ -8565,9 +8458,7 @@
         <v>325</v>
       </c>
       <c r="G79" s="25"/>
-      <c r="H79" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H79" s="25"/>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
@@ -8587,9 +8478,7 @@
       </c>
       <c r="F80" s="25"/>
       <c r="G80" s="25"/>
-      <c r="H80" s="25" t="s">
-        <v>328</v>
-      </c>
+      <c r="H80" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
commit to run 10 scnearios
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4783" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4780" uniqueCount="533">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1645,9 +1645,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -10762,9 +10759,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
-        <v>533</v>
-      </c>
+      <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="11" t="s">
@@ -10784,9 +10779,7 @@
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="1" t="s">
-        <v>532</v>
-      </c>
+      <c r="H43" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Updating the invokation listner
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C9639B4F-CFDA-4E15-9136-D215B4F1D053}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{1AE855E4-E569-4264-8B93-31716486F88B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="15" firstSheet="15" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="DriverSheet" r:id="rId1" sheetId="2"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5315" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5323" uniqueCount="547">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -11588,7 +11588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB81825B-AC84-43BA-896B-AD045DB7862F}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -12427,7 +12427,7 @@
       <c r="D41" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="26" t="s">
         <v>541</v>
       </c>
       <c r="F41" s="25" t="s">
@@ -12676,7 +12676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D77694-076F-429F-BF53-870C5B748F6D}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Check in to run the final cases
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,29 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{1AE855E4-E569-4264-8B93-31716486F88B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{995C1696-FA64-4A77-8AED-E7083F9D54F5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="15" firstSheet="15" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="4" firstSheet="4" tabRatio="500" windowHeight="10920" windowWidth="20490" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="600"/>
   </bookViews>
   <sheets>
     <sheet name="DriverSheet" r:id="rId1" sheetId="2"/>
     <sheet name="EngineGeneration" r:id="rId2" sheetId="19"/>
     <sheet name="VerifyCSVForExistingVersion" r:id="rId3" sheetId="3"/>
     <sheet name="VerifyCSVForNewVersion" r:id="rId4" sheetId="4"/>
-    <sheet name="VerifyDeleteOffer" r:id="rId5" sheetId="5"/>
-    <sheet name="VerifyEventAPI" r:id="rId6" sheetId="6"/>
-    <sheet name="VerifyRealtimeSpineAPI" r:id="rId7" sheetId="7"/>
-    <sheet name="RealtimeSpineWithNewProperty" r:id="rId8" sheetId="10"/>
-    <sheet name="EmailTempWithNewAttribute" r:id="rId9" sheetId="11"/>
-    <sheet name="MicrositeTempWithExistingAttrib" r:id="rId10" sheetId="12"/>
-    <sheet name="OBCCTempWithExistingAttrib" r:id="rId11" sheetId="17"/>
-    <sheet name="VerifyDBForNewAgreementModel" r:id="rId12" sheetId="13"/>
-    <sheet name="VerifyAgreementClassFornewProp" r:id="rId13" sheetId="14"/>
-    <sheet name="VerifyDiscardVersioIsSuccessful" r:id="rId14" sheetId="15"/>
-    <sheet name="EnsureRollbackIsSuccessful" r:id="rId15" sheetId="16"/>
-    <sheet name="AdpativeModelForUnsubscribe" r:id="rId16" sheetId="18"/>
-    <sheet name="BatchDecisionOutputValidations" r:id="rId17" sheetId="8"/>
-    <sheet name="CheckLists" r:id="rId18" sheetId="9"/>
+    <sheet name="VerifyIHDeleted" r:id="rId5" sheetId="20"/>
+    <sheet name="VerifyDeleteOffer" r:id="rId6" sheetId="5"/>
+    <sheet name="VerifyEventAPI" r:id="rId7" sheetId="6"/>
+    <sheet name="VerifyRealtimeSpineAPI" r:id="rId8" sheetId="7"/>
+    <sheet name="RealtimeSpineWithNewProperty" r:id="rId9" sheetId="10"/>
+    <sheet name="EmailTempWithNewAttribute" r:id="rId10" sheetId="11"/>
+    <sheet name="MicrositeTempWithExistingAttrib" r:id="rId11" sheetId="12"/>
+    <sheet name="OBCCTempWithExistingAttrib" r:id="rId12" sheetId="17"/>
+    <sheet name="VerifyDBForNewAgreementModel" r:id="rId13" sheetId="13"/>
+    <sheet name="VerifyAgreementClassFornewProp" r:id="rId14" sheetId="14"/>
+    <sheet name="VerifyDiscardVersioIsSuccessful" r:id="rId15" sheetId="15"/>
+    <sheet name="EnsureRollbackIsSuccessful" r:id="rId16" sheetId="16"/>
+    <sheet name="AdpativeModelForUnsubscribe" r:id="rId17" sheetId="18"/>
+    <sheet name="BatchDecisionOutputValidations" r:id="rId18" sheetId="8"/>
+    <sheet name="CheckLists" r:id="rId19" sheetId="9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5323" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5460" uniqueCount="558">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1687,10 +1688,43 @@
     <t>EngineGeneration</t>
   </si>
   <si>
-    <t>engine run multiple times</t>
+    <t>AdpativeModelForUnsubscribe</t>
+  </si>
+  <si>
+    <t>radPreviousrun</t>
+  </si>
+  <si>
+    <t>TS16_Regr_01</t>
+  </si>
+  <si>
+    <t>VerifyIHDeleted</t>
+  </si>
+  <si>
+    <t>Verifying the adaptive model for -ve response</t>
+  </si>
+  <si>
+    <t>Engine run multiple times</t>
+  </si>
+  <si>
+    <t>Clearing by Áll, verify IH deleted</t>
+  </si>
+  <si>
+    <t>lnkInteractionHistory</t>
+  </si>
+  <si>
+    <t>verifyIHRecordsAreAvailable</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>radioBtnAllForIH</t>
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -2381,10 +2415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2642,12 +2676,42 @@
         <v>544</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2660,6 +2724,1620 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162B974F-EC20-4DA5-9D9F-A5ACD05AB2C7}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:I77"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="42" t="s">
+        <v>405</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>488</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="9">
+        <v>7000</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="F24" s="25">
+        <v>2</v>
+      </c>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>369</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>370</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="31"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="30" t="s">
+        <v>375</v>
+      </c>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="F34" s="25">
+        <v>3</v>
+      </c>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="9"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="9"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F53" s="13">
+        <v>43525</v>
+      </c>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="9"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B56" s="36" t="s">
+        <v>383</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="D56" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" s="36" t="s">
+        <v>435</v>
+      </c>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B57" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="36"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B58" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>438</v>
+      </c>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F59" s="36"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="B60" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" s="36"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F61" s="29" t="s">
+        <v>368</v>
+      </c>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>391</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="F62" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="C63" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="D63" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="F63" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F65" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" s="9"/>
+      <c r="G66" s="25"/>
+      <c r="H66" s="25"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F67" s="9">
+        <v>10000</v>
+      </c>
+      <c r="G67" s="25"/>
+      <c r="H67" s="25"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" s="9"/>
+      <c r="G68" s="25"/>
+      <c r="H68" s="25"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" s="9"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="25"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="25"/>
+      <c r="H71" s="25"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F72" s="1">
+        <v>7000</v>
+      </c>
+      <c r="G72" s="25"/>
+      <c r="H72" s="25"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="25"/>
+      <c r="H73" s="25"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="25"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F75" s="33">
+        <v>30000</v>
+      </c>
+      <c r="G75" s="25"/>
+      <c r="H75" s="25"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G76" s="25"/>
+      <c r="H76" s="25"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CE6C41-C6E4-4D12-92D1-A13E0879FD5B}">
   <dimension ref="A1:I78"/>
   <sheetViews>
@@ -4290,7 +5968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DC9284-1E00-457F-9E32-CE2FA20C3859}">
   <sheetPr>
     <tabColor theme="4"/>
@@ -4739,12 +6417,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92316FED-85B2-43F2-9827-12AFBA752185}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:E51"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5110,9 +6788,7 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
@@ -5685,7 +7361,7 @@
         <v>279</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>278</v>
+        <v>546</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>254</v>
@@ -5855,12 +7531,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDE53E4-1746-48CE-AB4D-617AE971D39B}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6225,9 +7901,7 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
@@ -7244,12 +8918,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B88A9-98DC-469F-B6A8-72D4BD0DF47F}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7615,9 +9289,7 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
@@ -9160,12 +10832,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D209F-F23A-4BBD-9C0E-30D3275A1C3F}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9529,9 +11201,7 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
@@ -10883,9 +12553,7 @@
       <c r="E83" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F83" s="9">
-        <v>60</v>
-      </c>
+      <c r="F83" s="9"/>
       <c r="G83" s="25"/>
       <c r="H83" s="25"/>
     </row>
@@ -11584,12 +13252,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB81825B-AC84-43BA-896B-AD045DB7862F}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12076,7 +13744,9 @@
       <c r="E24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="25"/>
+      <c r="F24" s="25">
+        <v>5000</v>
+      </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
     </row>
@@ -12136,7 +13806,9 @@
       <c r="E27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="25"/>
+      <c r="F27" s="25">
+        <v>5000</v>
+      </c>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
     </row>
@@ -12156,7 +13828,9 @@
       <c r="E28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="25"/>
+      <c r="F28" s="25" t="s">
+        <v>204</v>
+      </c>
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
     </row>
@@ -12367,7 +14041,7 @@
         <v>280</v>
       </c>
       <c r="F38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
@@ -12447,7 +14121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
@@ -12635,7 +14309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:C3"/>
   <sheetViews>
@@ -12676,13 +14350,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D77694-076F-429F-BF53-870C5B748F6D}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
@@ -12769,9 +14443,7 @@
         <v>34</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -12793,9 +14465,7 @@
         <v>34</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
@@ -12817,9 +14487,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
@@ -12839,9 +14507,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
@@ -12863,9 +14529,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
@@ -12885,9 +14549,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
@@ -12909,9 +14571,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
@@ -12931,9 +14591,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
@@ -12955,9 +14613,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
@@ -12977,9 +14633,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
@@ -13001,9 +14655,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
@@ -13025,9 +14677,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -13047,9 +14697,7 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
@@ -13067,13 +14715,9 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>16</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="11" t="s">
@@ -13095,9 +14739,7 @@
         <v>5000</v>
       </c>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="11" t="s">
@@ -13117,9 +14759,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="11" t="s">
@@ -13141,9 +14781,7 @@
         <v>71</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="11" t="s">
@@ -13165,9 +14803,7 @@
         <v>75</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="11" t="s">
@@ -13187,9 +14823,7 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="11" t="s">
@@ -13211,9 +14845,7 @@
         <v>3000</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="11" t="s">
@@ -13233,9 +14865,7 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="11" t="s">
@@ -13255,9 +14885,7 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="11" t="s">
@@ -13277,9 +14905,7 @@
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="11" t="s">
@@ -13299,9 +14925,7 @@
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="11" t="s">
@@ -13321,9 +14945,7 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="11" t="s">
@@ -13343,9 +14965,7 @@
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="19" t="s">
@@ -13365,9 +14985,7 @@
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="11" t="s">
@@ -13387,9 +15005,7 @@
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="11" t="s">
@@ -13411,9 +15027,7 @@
         <v>3000</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="11" t="s">
@@ -13433,9 +15047,7 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="11" t="s">
@@ -13457,9 +15069,7 @@
         <v>3000</v>
       </c>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="11" t="s">
@@ -13479,9 +15089,7 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="11" t="s">
@@ -13503,9 +15111,7 @@
         <v>3000</v>
       </c>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="11" t="s">
@@ -13525,9 +15131,7 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="11" t="s">
@@ -13547,9 +15151,7 @@
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
-      <c r="H39" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="11" t="s">
@@ -13569,9 +15171,7 @@
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1" t="s">
-        <v>546</v>
-      </c>
+      <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="11" t="s">
@@ -13593,9 +15193,7 @@
         <v>30000</v>
       </c>
       <c r="G41" s="25"/>
-      <c r="H41" s="25" t="s">
-        <v>546</v>
-      </c>
+      <c r="H41" s="25"/>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="11" t="s">
@@ -13615,9 +15213,7 @@
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="25"/>
-      <c r="H42" s="25" t="s">
-        <v>546</v>
-      </c>
+      <c r="H42" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -13634,8 +15230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="C49" sqref="C49:F50"/>
+    <sheetView topLeftCell="A25" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14002,9 +15598,7 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="1"/>
     </row>
@@ -14683,8 +16277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A40" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15050,9 +16644,7 @@
       <c r="E18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
@@ -16083,6 +17675,713 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440AE6C1-8303-4801-938E-D5D89C6CD179}">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>553</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>522</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="F21" s="35"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>555</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F29" s="1">
+        <v>2</v>
+      </c>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>553</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>521</v>
+      </c>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
@@ -17213,12 +19512,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView topLeftCell="A9" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D16" sqref="D16:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17687,9 +19986,7 @@
       <c r="E23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
@@ -19015,14 +21312,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0" zoomScaleNormal="100">
+    <sheetView topLeftCell="A73" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -20747,7 +23044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F1A5F4-9176-42F8-9D13-5A98D8683A92}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -22826,1620 +25123,4 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162B974F-EC20-4DA5-9D9F-A5ACD05AB2C7}">
-  <sheetPr>
-    <tabColor theme="5"/>
-  </sheetPr>
-  <dimension ref="A1:I77"/>
-  <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70:E70"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="41.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="42" t="s">
-        <v>405</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="9">
-        <v>2000</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="9">
-        <v>3000</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="9">
-        <v>3000</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="9">
-        <v>3000</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>530</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>488</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="9">
-        <v>93</v>
-      </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="9">
-        <v>7000</v>
-      </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="9"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>357</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>359</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>358</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="27" t="s">
-        <v>361</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>360</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>362</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="F24" s="25">
-        <v>2</v>
-      </c>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>364</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>363</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>366</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>367</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>368</v>
-      </c>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>369</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>370</v>
-      </c>
-      <c r="E27" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="F27" s="31"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>371</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>372</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>375</v>
-      </c>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="15" t="s">
-        <v>355</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>373</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>374</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>376</v>
-      </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>377</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>378</v>
-      </c>
-      <c r="E30" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>357</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>379</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>358</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>244</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>280</v>
-      </c>
-      <c r="F34" s="25">
-        <v>3</v>
-      </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F47" s="9"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F48" s="9"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F49" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="9"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B51" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B53" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F53" s="13">
-        <v>43525</v>
-      </c>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F54" s="13">
-        <v>45719</v>
-      </c>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="9"/>
-      <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="B56" s="36" t="s">
-        <v>383</v>
-      </c>
-      <c r="C56" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="D56" s="20" t="s">
-        <v>434</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F56" s="36" t="s">
-        <v>435</v>
-      </c>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="B57" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="C57" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>436</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="36"/>
-      <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="B58" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="C58" s="20" t="s">
-        <v>439</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="F58" s="36" t="s">
-        <v>438</v>
-      </c>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="B59" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="C59" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>441</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F59" s="36"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="B60" s="36" t="s">
-        <v>384</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F60" s="36"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B61" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F61" s="29" t="s">
-        <v>368</v>
-      </c>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="C62" s="26" t="s">
-        <v>391</v>
-      </c>
-      <c r="D62" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="F62" s="27" t="s">
-        <v>375</v>
-      </c>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>390</v>
-      </c>
-      <c r="C63" s="26" t="s">
-        <v>392</v>
-      </c>
-      <c r="D63" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="26" t="s">
-        <v>393</v>
-      </c>
-      <c r="F63" s="27" t="s">
-        <v>376</v>
-      </c>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F65" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F66" s="9"/>
-      <c r="G66" s="25"/>
-      <c r="H66" s="25"/>
-    </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F67" s="9">
-        <v>10000</v>
-      </c>
-      <c r="G67" s="25"/>
-      <c r="H67" s="25"/>
-    </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F68" s="9"/>
-      <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F69" s="9"/>
-      <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>401</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="F70" s="1"/>
-      <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D72" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" s="1">
-        <v>7000</v>
-      </c>
-      <c r="G72" s="25"/>
-      <c r="H72" s="25"/>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F73" s="1"/>
-      <c r="G73" s="25"/>
-      <c r="H73" s="25"/>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="25"/>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F75" s="33">
-        <v>30000</v>
-      </c>
-      <c r="G75" s="25"/>
-      <c r="H75" s="25"/>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F77" s="1"/>
-      <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Check in to verify the timeout issue
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{995C1696-FA64-4A77-8AED-E7083F9D54F5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{3935C56B-5C95-4850-B295-9F1E67CC98AE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="4" firstSheet="4" tabRatio="500" windowHeight="10920" windowWidth="20490" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="600"/>
+    <workbookView activeTab="5" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="DriverSheet" r:id="rId1" sheetId="2"/>
-    <sheet name="EngineGeneration" r:id="rId2" sheetId="19"/>
-    <sheet name="VerifyCSVForExistingVersion" r:id="rId3" sheetId="3"/>
-    <sheet name="VerifyCSVForNewVersion" r:id="rId4" sheetId="4"/>
-    <sheet name="VerifyIHDeleted" r:id="rId5" sheetId="20"/>
-    <sheet name="VerifyDeleteOffer" r:id="rId6" sheetId="5"/>
+    <sheet name="VerifyCSVForExistingVersion" r:id="rId2" sheetId="3"/>
+    <sheet name="VerifyCSVForNewVersion" r:id="rId3" sheetId="4"/>
+    <sheet name="VerifyIHDeleted" r:id="rId4" sheetId="20"/>
+    <sheet name="VerifyDeleteOffer" r:id="rId5" sheetId="5"/>
+    <sheet name="RenameOffer" r:id="rId6" sheetId="21"/>
     <sheet name="VerifyEventAPI" r:id="rId7" sheetId="6"/>
     <sheet name="VerifyRealtimeSpineAPI" r:id="rId8" sheetId="7"/>
     <sheet name="RealtimeSpineWithNewProperty" r:id="rId9" sheetId="10"/>
@@ -33,7 +33,7 @@
     <sheet name="BatchDecisionOutputValidations" r:id="rId18" sheetId="8"/>
     <sheet name="CheckLists" r:id="rId19" sheetId="9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5460" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5522" uniqueCount="566">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1682,12 +1682,6 @@
     <t>Negative</t>
   </si>
   <si>
-    <t>generate engine</t>
-  </si>
-  <si>
-    <t>EngineGeneration</t>
-  </si>
-  <si>
     <t>AdpativeModelForUnsubscribe</t>
   </si>
   <si>
@@ -1703,9 +1697,6 @@
     <t>Verifying the adaptive model for -ve response</t>
   </si>
   <si>
-    <t>Engine run multiple times</t>
-  </si>
-  <si>
     <t>Clearing by Áll, verify IH deleted</t>
   </si>
   <si>
@@ -1719,6 +1710,39 @@
   </si>
   <si>
     <t>radioBtnAllForIH</t>
+  </si>
+  <si>
+    <t>Scenario to verify the rename offer is successful or not</t>
+  </si>
+  <si>
+    <t>TS1_Regr_03</t>
+  </si>
+  <si>
+    <t>New offer to rename</t>
+  </si>
+  <si>
+    <t>NewOfferToRename</t>
+  </si>
+  <si>
+    <t>enableOverride</t>
+  </si>
+  <si>
+    <t>RenameOffer</t>
+  </si>
+  <si>
+    <t>Verify renaming of offer is successful</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>increaseWeightIfRequired</t>
+  </si>
+  <si>
+    <t>select override for the offer</t>
+  </si>
+  <si>
+    <t>drag to top if below in the list</t>
   </si>
   <si>
     <t>Pass</t>
@@ -2418,7 +2442,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2499,7 +2523,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -2514,7 +2538,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -2529,7 +2553,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2544,7 +2568,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -2559,7 +2583,7 @@
         <v>354</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -2574,7 +2598,7 @@
         <v>365</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -2589,7 +2613,7 @@
         <v>414</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -2604,7 +2628,7 @@
         <v>451</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -2619,7 +2643,7 @@
         <v>464</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -2634,7 +2658,7 @@
         <v>482</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -2649,7 +2673,7 @@
         <v>509</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -2664,49 +2688,49 @@
         <v>524</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="25" t="s">
-        <v>0</v>
+      <c r="A18" s="1" t="s">
+        <v>532</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
-        <v>532</v>
+        <v>545</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>560</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>548</v>
+        <v>558</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>551</v>
+        <v>559</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -7361,7 +7385,7 @@
         <v>279</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E46" s="20" t="s">
         <v>254</v>
@@ -14347,891 +14371,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D77694-076F-429F-BF53-870C5B748F6D}">
-  <dimension ref="A1:I42"/>
-  <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="9">
-        <v>2000</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="9">
-        <v>3000</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="9">
-        <v>3000</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="9">
-        <v>3000</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>528</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>488</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="1">
-        <v>5000</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F33" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F35" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="1">
-        <v>30000</v>
-      </c>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" s="1"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16273,12 +15417,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C53" sqref="C53:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17674,11 +16818,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440AE6C1-8303-4801-938E-D5D89C6CD179}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -17754,7 +16898,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>32</v>
@@ -17770,13 +16914,11 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
@@ -17794,13 +16936,11 @@
         <v>34</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>39</v>
@@ -17818,13 +16958,11 @@
         <v>5000</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>42</v>
@@ -17840,13 +16978,11 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>46</v>
@@ -17864,13 +17000,11 @@
         <v>162</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>47</v>
@@ -17886,13 +17020,11 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>50</v>
@@ -17910,13 +17042,11 @@
         <v>163</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>51</v>
@@ -17932,13 +17062,11 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>54</v>
@@ -17956,13 +17084,11 @@
         <v>163</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>55</v>
@@ -17978,13 +17104,11 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>58</v>
@@ -18002,13 +17126,11 @@
         <v>163</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>61</v>
@@ -18026,19 +17148,17 @@
         <v>60</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>146</v>
@@ -18048,19 +17168,17 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>34</v>
@@ -18072,65 +17190,59 @@
         <v>5000</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>556</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F20" s="37" t="s">
         <v>522</v>
       </c>
       <c r="G20" s="25"/>
-      <c r="H20" s="25" t="s">
-        <v>557</v>
-      </c>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>34</v>
@@ -18144,13 +17256,13 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>178</v>
@@ -18164,13 +17276,13 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>34</v>
@@ -18186,16 +17298,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E24" s="20" t="s">
         <v>254</v>
@@ -18206,13 +17318,13 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>181</v>
@@ -18226,13 +17338,13 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>34</v>
@@ -18246,13 +17358,13 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>534</v>
@@ -18266,13 +17378,13 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>34</v>
@@ -18288,13 +17400,13 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>34</v>
@@ -18310,13 +17422,13 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>146</v>
@@ -18330,16 +17442,16 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>45</v>
@@ -18350,19 +17462,19 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="F32" s="37" t="s">
         <v>521</v>
@@ -18381,7 +17493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I54"/>
   <sheetViews>
@@ -19509,6 +18621,1155 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
   <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFAFDA0-4A55-4936-A3DC-B19DEB90A342}">
+  <dimension ref="A1:I53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="42" t="s">
+        <v>553</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>488</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="9">
+        <v>7000</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="9" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="9" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="13">
+        <v>43525</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="13">
+        <v>45719</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>433</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>435</v>
+      </c>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" s="20" t="s">
+        <v>436</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" s="36"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>439</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>437</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" s="36" t="s">
+        <v>438</v>
+      </c>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="D44" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="36"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" s="36"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F49" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" s="9"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F51" s="9">
+        <v>10000</v>
+      </c>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Check in to run full suite
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{3935C56B-5C95-4850-B295-9F1E67CC98AE}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BD8C921D-65F4-456E-B6E9-85AD7B390B1E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43"/>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="3" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView activeTab="15" firstSheet="14" tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="DriverSheet" r:id="rId1" sheetId="2"/>
@@ -33,7 +33,7 @@
     <sheet name="BatchDecisionOutputValidations" r:id="rId18" sheetId="8"/>
     <sheet name="CheckLists" r:id="rId19" sheetId="9"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5522" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5909" uniqueCount="594">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1733,22 +1733,106 @@
     <t>Verify renaming of offer is successful</t>
   </si>
   <si>
+    <t>increaseWeightIfRequired</t>
+  </si>
+  <si>
+    <t>select override for the offer</t>
+  </si>
+  <si>
+    <t>drag to top if below in the list</t>
+  </si>
+  <si>
+    <t>Define brain</t>
+  </si>
+  <si>
+    <t>switch to parent frame</t>
+  </si>
+  <si>
+    <t>click toggle navigation</t>
+  </si>
+  <si>
+    <t>Renaming offer</t>
+  </si>
+  <si>
+    <t>radBtnUpdateOffer</t>
+  </si>
+  <si>
+    <t>TS_65</t>
+  </si>
+  <si>
+    <t>TS_66</t>
+  </si>
+  <si>
+    <t>TS_67</t>
+  </si>
+  <si>
+    <t>TS_68</t>
+  </si>
+  <si>
+    <t>TS_69</t>
+  </si>
+  <si>
+    <t>TS_70</t>
+  </si>
+  <si>
+    <t>TS_71</t>
+  </si>
+  <si>
+    <t>TS_72</t>
+  </si>
+  <si>
+    <t>TS_73</t>
+  </si>
+  <si>
+    <t>TS_74</t>
+  </si>
+  <si>
+    <t>TS_75</t>
+  </si>
+  <si>
+    <t>TS_76</t>
+  </si>
+  <si>
+    <t>TS_77</t>
+  </si>
+  <si>
+    <t>TS_78</t>
+  </si>
+  <si>
+    <t>TS_79</t>
+  </si>
+  <si>
+    <t>TS_80</t>
+  </si>
+  <si>
+    <t>TS_81</t>
+  </si>
+  <si>
+    <t>TS_82</t>
+  </si>
+  <si>
+    <t>TS_83</t>
+  </si>
+  <si>
+    <t>TS_84</t>
+  </si>
+  <si>
+    <t>RenamedOfferQA</t>
+  </si>
+  <si>
+    <t>ddnSubChannel</t>
+  </si>
+  <si>
+    <t>select subchannel</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>increaseWeightIfRequired</t>
-  </si>
-  <si>
-    <t>select override for the offer</t>
-  </si>
-  <si>
-    <t>drag to top if below in the list</t>
+    <t>DirectMailUK</t>
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -2442,7 +2526,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2508,7 +2592,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -2523,7 +2607,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -2537,8 +2621,8 @@
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>560</v>
+      <c r="D7" s="20" t="s">
+        <v>591</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -2553,7 +2637,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2567,8 +2651,8 @@
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>560</v>
+      <c r="D9" s="20" t="s">
+        <v>591</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -2582,8 +2666,8 @@
       <c r="C10" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>560</v>
+      <c r="D10" s="20" t="s">
+        <v>591</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -2598,7 +2682,7 @@
         <v>365</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -2613,7 +2697,7 @@
         <v>414</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -2628,7 +2712,7 @@
         <v>451</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -2643,7 +2727,7 @@
         <v>464</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -2658,7 +2742,7 @@
         <v>482</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>560</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -2673,7 +2757,7 @@
         <v>509</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -2688,7 +2772,7 @@
         <v>524</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -2703,7 +2787,7 @@
         <v>547</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -2718,7 +2802,7 @@
         <v>548</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>560</v>
+        <v>591</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -2733,7 +2817,7 @@
         <v>559</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -2752,10 +2836,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4209,18 +4293,20 @@
         <v>355</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F71" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F71" s="9">
+        <v>3000</v>
+      </c>
       <c r="G71" s="25"/>
       <c r="H71" s="25"/>
     </row>
@@ -4229,20 +4315,18 @@
         <v>355</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>279</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F72" s="1">
-        <v>7000</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="25"/>
       <c r="H72" s="25"/>
     </row>
@@ -4251,18 +4335,20 @@
         <v>355</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>106</v>
+        <v>279</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F73" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="F73" s="1">
+        <v>7000</v>
+      </c>
       <c r="G73" s="25"/>
       <c r="H73" s="25"/>
     </row>
@@ -4274,15 +4360,15 @@
         <v>404</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F74" s="25"/>
+      <c r="F74" s="1"/>
       <c r="G74" s="25"/>
       <c r="H74" s="25"/>
     </row>
@@ -4294,17 +4380,15 @@
         <v>404</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F75" s="33">
-        <v>30000</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F75" s="25"/>
       <c r="G75" s="25"/>
       <c r="H75" s="25"/>
     </row>
@@ -4316,16 +4400,16 @@
         <v>404</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>203</v>
+        <v>40</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>204</v>
+        <v>41</v>
+      </c>
+      <c r="F76" s="33">
+        <v>30000</v>
       </c>
       <c r="G76" s="25"/>
       <c r="H76" s="25"/>
@@ -4338,17 +4422,39 @@
         <v>404</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>406</v>
+        <v>203</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F77" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="G77" s="25"/>
       <c r="H77" s="25"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F78" s="1"/>
+      <c r="G78" s="25"/>
+      <c r="H78" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6446,7 +6552,7 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D44" sqref="D44:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7559,7 +7665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDE53E4-1746-48CE-AB4D-617AE971D39B}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -8944,10 +9050,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B88A9-98DC-469F-B6A8-72D4BD0DF47F}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9041,7 +9147,9 @@
         <v>34</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -9063,7 +9171,9 @@
         <v>34</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -9085,7 +9195,9 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -9105,7 +9217,9 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -9127,7 +9241,9 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -9147,7 +9263,9 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -9169,7 +9287,9 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -9189,7 +9309,9 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -9211,7 +9333,9 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+      <c r="H13" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -9231,7 +9355,9 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -9253,7 +9379,9 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
+      <c r="H15" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -9275,7 +9403,9 @@
         <v>60</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="H16" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -9295,7 +9425,9 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="H17" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -9315,7 +9447,9 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="H18" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -9337,7 +9471,9 @@
         <v>7000</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="H19" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -9357,7 +9493,9 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -9379,7 +9517,9 @@
         <v>478</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="9"/>
+      <c r="H21" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -9401,7 +9541,9 @@
         <v>478</v>
       </c>
       <c r="G22" s="1"/>
-      <c r="H22" s="9"/>
+      <c r="H22" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -9421,7 +9563,9 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="9"/>
+      <c r="H23" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -9443,7 +9587,9 @@
         <v>3000</v>
       </c>
       <c r="G24" s="1"/>
-      <c r="H24" s="9"/>
+      <c r="H24" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -9463,7 +9609,9 @@
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="9"/>
+      <c r="H25" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -9483,7 +9631,9 @@
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
+      <c r="H26" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -9503,7 +9653,9 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
+      <c r="H27" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -9523,7 +9675,9 @@
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
+      <c r="H28" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -9543,7 +9697,9 @@
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
+      <c r="H29" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -9563,7 +9719,9 @@
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -9583,7 +9741,9 @@
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
+      <c r="H31" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -9603,7 +9763,9 @@
       </c>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
+      <c r="H32" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -9623,7 +9785,9 @@
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
+      <c r="H33" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -9645,7 +9809,9 @@
         <v>494</v>
       </c>
       <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
+      <c r="H34" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -9665,7 +9831,9 @@
       </c>
       <c r="F35" s="25"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
+      <c r="H35" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -9685,7 +9853,9 @@
       </c>
       <c r="F36" s="25"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
+      <c r="H36" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -9707,7 +9877,9 @@
         <v>7000</v>
       </c>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
+      <c r="H37" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -9727,7 +9899,9 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
+      <c r="H38" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -9749,7 +9923,9 @@
         <v>3000</v>
       </c>
       <c r="G39" s="1"/>
-      <c r="H39" s="9"/>
+      <c r="H39" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -9773,7 +9949,9 @@
       <c r="G40" s="1" t="s">
         <v>494</v>
       </c>
-      <c r="H40" s="9"/>
+      <c r="H40" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -9793,7 +9971,9 @@
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
+      <c r="H41" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -9813,7 +9993,9 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="H42" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -9835,7 +10017,9 @@
         <v>479</v>
       </c>
       <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
+      <c r="H43" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -9857,7 +10041,9 @@
         <v>43525</v>
       </c>
       <c r="G44" s="13"/>
-      <c r="H44" s="9"/>
+      <c r="H44" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -9879,7 +10065,9 @@
         <v>45719</v>
       </c>
       <c r="G45" s="13"/>
-      <c r="H45" s="9"/>
+      <c r="H45" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -9899,7 +10087,9 @@
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
+      <c r="H46" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -9921,7 +10111,9 @@
         <v>435</v>
       </c>
       <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
+      <c r="H47" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -9941,7 +10133,9 @@
       </c>
       <c r="F48" s="36"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -9963,7 +10157,9 @@
         <v>438</v>
       </c>
       <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
+      <c r="H49" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -9983,7 +10179,9 @@
       </c>
       <c r="F50" s="36"/>
       <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
+      <c r="H50" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -10003,7 +10201,9 @@
       </c>
       <c r="F51" s="36"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
+      <c r="H51" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -10023,7 +10223,9 @@
       </c>
       <c r="F52" s="36"/>
       <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
+      <c r="H52" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -10043,7 +10245,9 @@
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
+      <c r="H53" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -10065,7 +10269,9 @@
         <v>150</v>
       </c>
       <c r="G54" s="1"/>
-      <c r="H54" s="9"/>
+      <c r="H54" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -10085,7 +10291,9 @@
       </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
-      <c r="H55" s="9"/>
+      <c r="H55" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -10107,48 +10315,48 @@
         <v>155</v>
       </c>
       <c r="G56" s="1"/>
-      <c r="H56" s="9"/>
+      <c r="H56" s="9" t="s">
+        <v>593</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
-      <c r="A57" s="1" t="s">
-        <v>481</v>
-      </c>
+      <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="F57" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G57" s="1"/>
       <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="1" t="s">
-        <v>481</v>
-      </c>
+      <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>34</v>
+        <v>589</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F58" s="1">
-        <v>5000</v>
-      </c>
-      <c r="G58" s="9"/>
+        <v>149</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="G58" s="1"/>
       <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8">
@@ -10156,16 +10364,16 @@
         <v>481</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>34</v>
+        <v>157</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>34</v>
+        <v>144</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>486</v>
+        <v>45</v>
       </c>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
@@ -10176,60 +10384,60 @@
         <v>481</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C60" s="26" t="s">
-        <v>483</v>
-      </c>
-      <c r="D60" s="26" t="s">
-        <v>484</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>452</v>
-      </c>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
+        <v>160</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F60" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>481</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>161</v>
+        <v>34</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+        <v>486</v>
+      </c>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>481</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="1">
-        <v>5000</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="C62" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="E62" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="F62" s="25"/>
       <c r="G62" s="25"/>
       <c r="H62" s="25"/>
     </row>
@@ -10238,18 +10446,18 @@
         <v>481</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>339</v>
+        <v>172</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>487</v>
+        <v>161</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F63" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F63" s="25"/>
       <c r="G63" s="25"/>
       <c r="H63" s="25"/>
     </row>
@@ -10258,18 +10466,20 @@
         <v>481</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C64" s="27" t="s">
-        <v>359</v>
-      </c>
-      <c r="D64" s="27" t="s">
-        <v>358</v>
-      </c>
-      <c r="E64" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="F64" s="25"/>
+        <v>338</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F64" s="1">
+        <v>5000</v>
+      </c>
       <c r="G64" s="25"/>
       <c r="H64" s="25"/>
     </row>
@@ -10278,18 +10488,18 @@
         <v>481</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C65" s="25" t="s">
-        <v>485</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F65" s="25"/>
+        <v>339</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F65" s="1"/>
       <c r="G65" s="25"/>
       <c r="H65" s="25"/>
     </row>
@@ -10298,20 +10508,18 @@
         <v>481</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>163</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="C66" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="D66" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" s="25"/>
       <c r="G66" s="25"/>
       <c r="H66" s="25"/>
     </row>
@@ -10322,18 +10530,16 @@
       <c r="B67" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>34</v>
+      <c r="C67" s="25" t="s">
+        <v>485</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>186</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F67" s="25"/>
       <c r="G67" s="25"/>
       <c r="H67" s="25"/>
     </row>
@@ -10342,18 +10548,20 @@
         <v>481</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="C68" s="26" t="s">
-        <v>489</v>
-      </c>
-      <c r="D68" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="26" t="s">
-        <v>488</v>
-      </c>
-      <c r="F68" s="25"/>
+        <v>341</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="G68" s="25"/>
       <c r="H68" s="25"/>
     </row>
@@ -10362,19 +10570,19 @@
         <v>481</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="C69" s="25" t="s">
-        <v>490</v>
+        <v>341</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F69" s="1">
-        <v>5000</v>
+      <c r="E69" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="G69" s="25"/>
       <c r="H69" s="25"/>
@@ -10384,18 +10592,18 @@
         <v>481</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="C70" s="25" t="s">
-        <v>491</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F70" s="1"/>
+        <v>343</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>489</v>
+      </c>
+      <c r="D70" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>488</v>
+      </c>
+      <c r="F70" s="25"/>
       <c r="G70" s="25"/>
       <c r="H70" s="25"/>
     </row>
@@ -10404,19 +10612,19 @@
         <v>481</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>68</v>
+        <v>345</v>
+      </c>
+      <c r="C71" s="25" t="s">
+        <v>490</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>492</v>
+        <v>41</v>
+      </c>
+      <c r="F71" s="1">
+        <v>5000</v>
       </c>
       <c r="G71" s="25"/>
       <c r="H71" s="25"/>
@@ -10426,20 +10634,18 @@
         <v>481</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>73</v>
+        <v>346</v>
+      </c>
+      <c r="C72" s="25" t="s">
+        <v>491</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>492</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F72" s="1"/>
       <c r="G72" s="25"/>
       <c r="H72" s="25"/>
     </row>
@@ -10448,18 +10654,20 @@
         <v>481</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F73" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="G73" s="25"/>
       <c r="H73" s="25"/>
     </row>
@@ -10468,19 +10676,19 @@
         <v>481</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F74" s="1">
-        <v>7000</v>
+        <v>70</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>492</v>
       </c>
       <c r="G74" s="25"/>
       <c r="H74" s="25"/>
@@ -10490,7 +10698,7 @@
         <v>481</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>77</v>
@@ -10510,12 +10718,12 @@
         <v>481</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D76" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E76" s="1" t="s">
@@ -10532,12 +10740,12 @@
         <v>481</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D77" s="38" t="s">
+      <c r="D77" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E77" s="1" t="s">
@@ -10552,23 +10760,21 @@
         <v>481</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="D78" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="26" t="s">
-        <v>496</v>
-      </c>
-      <c r="F78" s="25" t="s">
-        <v>479</v>
-      </c>
-      <c r="G78" s="37" t="s">
-        <v>521</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F78" s="1">
+        <v>7000</v>
+      </c>
+      <c r="G78" s="25"/>
       <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
@@ -10576,23 +10782,19 @@
         <v>481</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="D79" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>495</v>
-      </c>
-      <c r="F79" s="26" t="s">
-        <v>499</v>
-      </c>
-      <c r="G79" s="26" t="s">
-        <v>494</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="25"/>
       <c r="H79" s="25"/>
     </row>
     <row r="80" spans="1:8">
@@ -10600,21 +10802,23 @@
         <v>481</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="D80" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F80" s="25">
-        <v>7000</v>
-      </c>
-      <c r="G80" s="25"/>
+      <c r="D80" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="26" t="s">
+        <v>496</v>
+      </c>
+      <c r="F80" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="G80" s="37" t="s">
+        <v>521</v>
+      </c>
       <c r="H80" s="25"/>
     </row>
     <row r="81" spans="1:8">
@@ -10622,19 +10826,23 @@
         <v>481</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="D81" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F81" s="25"/>
-      <c r="G81" s="25"/>
+      <c r="D81" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="F81" s="26" t="s">
+        <v>499</v>
+      </c>
+      <c r="G81" s="26" t="s">
+        <v>494</v>
+      </c>
       <c r="H81" s="25"/>
     </row>
     <row r="82" spans="1:8">
@@ -10642,7 +10850,7 @@
         <v>481</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>497</v>
@@ -10664,13 +10872,13 @@
         <v>481</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>99</v>
+      <c r="D83" s="38" t="s">
+        <v>78</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>45</v>
@@ -10684,18 +10892,20 @@
         <v>481</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D84" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="F84" s="1"/>
+        <v>497</v>
+      </c>
+      <c r="D84" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F84" s="25">
+        <v>7000</v>
+      </c>
       <c r="G84" s="25"/>
       <c r="H84" s="25"/>
     </row>
@@ -10704,18 +10914,18 @@
         <v>481</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D85" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="E85" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F85" s="1"/>
+        <v>498</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" s="25"/>
       <c r="G85" s="25"/>
       <c r="H85" s="25"/>
     </row>
@@ -10724,20 +10934,18 @@
         <v>481</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D86" s="20" t="s">
-        <v>34</v>
+        <v>498</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F86" s="1">
-        <v>7000</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F86" s="25"/>
       <c r="G86" s="25"/>
       <c r="H86" s="25"/>
     </row>
@@ -10749,13 +10957,13 @@
         <v>403</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>107</v>
+        <v>40</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="20" t="s">
+        <v>501</v>
       </c>
       <c r="F87" s="1"/>
       <c r="G87" s="25"/>
@@ -10769,15 +10977,15 @@
         <v>403</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F88" s="25"/>
+        <v>279</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="E88" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F88" s="1"/>
       <c r="G88" s="25"/>
       <c r="H88" s="25"/>
     </row>
@@ -10789,16 +10997,16 @@
         <v>403</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D89" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D89" s="20" t="s">
         <v>34</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F89" s="33">
-        <v>30000</v>
+      <c r="F89" s="1">
+        <v>7000</v>
       </c>
       <c r="G89" s="25"/>
       <c r="H89" s="25"/>
@@ -10811,17 +11019,15 @@
         <v>403</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>203</v>
+        <v>105</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>204</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F90" s="1"/>
       <c r="G90" s="25"/>
       <c r="H90" s="25"/>
     </row>
@@ -10833,17 +11039,81 @@
         <v>403</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>406</v>
+        <v>120</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F91" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="F91" s="25"/>
       <c r="G91" s="25"/>
       <c r="H91" s="25"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F92" s="33">
+        <v>30000</v>
+      </c>
+      <c r="G92" s="25"/>
+      <c r="H92" s="25"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G93" s="25"/>
+      <c r="H93" s="25"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F94" s="1"/>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10860,7 +11130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D209F-F23A-4BBD-9C0E-30D3275A1C3F}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
       <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
@@ -13280,8 +13550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB81825B-AC84-43BA-896B-AD045DB7862F}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:F28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14147,7 +14417,7 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D12" sqref="D12"/>
@@ -14320,6 +14590,40 @@
       </c>
       <c r="E10" s="18" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>556</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -14374,7 +14678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
+    <sheetView topLeftCell="A40" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
@@ -15419,10 +15723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="C53" sqref="C53:F56"/>
+    <sheetView topLeftCell="A43" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D51" sqref="D51:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16461,19 +16765,21 @@
         <v>14</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="F51" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G51" s="1"/>
       <c r="H51" s="9"/>
     </row>
     <row r="52" spans="1:8">
@@ -16481,21 +16787,21 @@
         <v>14</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>157</v>
+        <v>590</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>34</v>
+        <v>589</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F52" s="9">
-        <v>5000</v>
-      </c>
-      <c r="G52" s="9"/>
+        <v>149</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="G52" s="1"/>
       <c r="H52" s="9"/>
     </row>
     <row r="53" spans="1:8">
@@ -16503,13 +16809,13 @@
         <v>14</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>45</v>
@@ -16523,10 +16829,10 @@
         <v>14</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>40</v>
+        <v>157</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>34</v>
@@ -16535,7 +16841,7 @@
         <v>41</v>
       </c>
       <c r="F54" s="9">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
@@ -16545,13 +16851,13 @@
         <v>14</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>98</v>
+        <v>157</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>45</v>
@@ -16565,18 +16871,20 @@
         <v>14</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="9"/>
+        <v>41</v>
+      </c>
+      <c r="F56" s="9">
+        <v>10000</v>
+      </c>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
     </row>
@@ -16585,40 +16893,40 @@
         <v>14</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>254</v>
-      </c>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
+        <v>161</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
@@ -16628,17 +16936,15 @@
         <v>103</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>279</v>
+        <v>40</v>
       </c>
       <c r="D59" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59" s="1">
-        <v>7000</v>
-      </c>
+      <c r="E59" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
     </row>
@@ -16647,16 +16953,16 @@
         <v>14</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>107</v>
+        <v>279</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>254</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -16667,18 +16973,20 @@
         <v>14</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F61" s="1"/>
+        <v>279</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="1">
+        <v>7000</v>
+      </c>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
     </row>
@@ -16687,16 +16995,16 @@
         <v>14</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -16707,20 +17015,18 @@
         <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="1">
-        <v>10000</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
     </row>
@@ -16729,16 +17035,16 @@
         <v>14</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -16749,18 +17055,20 @@
         <v>14</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F65" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="F65" s="1">
+        <v>10000</v>
+      </c>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
     </row>
@@ -16769,20 +17077,18 @@
         <v>14</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>40</v>
+        <v>117</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="1">
-        <v>30000</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
     </row>
@@ -16791,20 +17097,62 @@
         <v>14</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>34</v>
+        <v>121</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F68" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16822,7 +17170,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440AE6C1-8303-4801-938E-D5D89C6CD179}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -17498,7 +17846,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView topLeftCell="A37" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="D44" sqref="D44:E44"/>
+      <selection activeCell="D38" sqref="D38:F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18626,10 +18974,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFAFDA0-4A55-4936-A3DC-B19DEB90A342}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18722,9 +19070,7 @@
         <v>34</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -18746,9 +19092,7 @@
         <v>34</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -18770,9 +19114,7 @@
         <v>5000</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -18792,9 +19134,7 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -18816,9 +19156,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -18838,9 +19176,7 @@
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -18862,9 +19198,7 @@
         <v>3000</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -18884,9 +19218,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -18908,9 +19240,7 @@
         <v>3000</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -18930,9 +19260,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -18954,9 +19282,7 @@
         <v>3000</v>
       </c>
       <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -18978,9 +19304,7 @@
         <v>60</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -19000,9 +19324,7 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -19022,9 +19344,7 @@
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -19046,9 +19366,7 @@
         <v>7000</v>
       </c>
       <c r="G19" s="9"/>
-      <c r="H19" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -19068,9 +19386,7 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="9" t="s">
-        <v>564</v>
-      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -19092,9 +19408,7 @@
         <v>555</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="9" t="s">
-        <v>565</v>
-      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -19726,7 +20040,7 @@
         <v>160</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>34</v>
@@ -19748,19 +20062,1085 @@
         <v>160</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>556</v>
       </c>
       <c r="G53" s="25"/>
       <c r="H53" s="25"/>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="25"/>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59" s="1">
+        <v>7000</v>
+      </c>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="25"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F62" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G62" s="25"/>
+      <c r="H62" s="25"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G63" s="25"/>
+      <c r="H63" s="25"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D64" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>185</v>
+      </c>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>565</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" s="9"/>
+      <c r="G66" s="25"/>
+      <c r="H66" s="25"/>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F67" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G67" s="25"/>
+      <c r="H67" s="25"/>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="F68" s="9">
+        <v>2</v>
+      </c>
+      <c r="G68" s="25"/>
+      <c r="H68" s="25"/>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="36" t="s">
+        <v>488</v>
+      </c>
+      <c r="F69" s="9"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="25"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="C70" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F70" s="25">
+        <v>5000</v>
+      </c>
+      <c r="G70" s="25"/>
+      <c r="H70" s="25"/>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C71" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" s="25"/>
+      <c r="G71" s="25"/>
+      <c r="H71" s="25"/>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="A72" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F72" s="25" t="s">
+        <v>566</v>
+      </c>
+      <c r="G72" s="25"/>
+      <c r="H72" s="25"/>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="A73" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C73" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" s="25" t="s">
+        <v>566</v>
+      </c>
+      <c r="G73" s="25"/>
+      <c r="H73" s="25"/>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C74" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="25"/>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C75" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F75" s="25">
+        <v>3000</v>
+      </c>
+      <c r="G75" s="25"/>
+      <c r="H75" s="25"/>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C76" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" s="25"/>
+      <c r="G76" s="25"/>
+      <c r="H76" s="25"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C77" s="26" t="s">
+        <v>564</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F77" s="25">
+        <v>3000</v>
+      </c>
+      <c r="G77" s="25"/>
+      <c r="H77" s="25"/>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="C78" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" s="25"/>
+      <c r="G78" s="25"/>
+      <c r="H78" s="25"/>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C79" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F79" s="1">
+        <v>8000</v>
+      </c>
+      <c r="G79" s="25"/>
+      <c r="H79" s="25"/>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="G80" s="25"/>
+      <c r="H80" s="25"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C81" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D81" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F81" s="25">
+        <v>8000</v>
+      </c>
+      <c r="G81" s="25"/>
+      <c r="H81" s="25"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C82" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D82" s="26" t="s">
+        <v>567</v>
+      </c>
+      <c r="E82" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" s="25"/>
+      <c r="G82" s="25"/>
+      <c r="H82" s="25"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="C83" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="G83" s="25"/>
+      <c r="H83" s="25"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C84" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D84" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F84" s="25">
+        <v>5000</v>
+      </c>
+      <c r="G84" s="25"/>
+      <c r="H84" s="25"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="G85" s="25"/>
+      <c r="H85" s="25"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="C86" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F86" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G86" s="25"/>
+      <c r="H86" s="25"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C87" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="1"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="25"/>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C88" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F88" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G88" s="25"/>
+      <c r="H88" s="25"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C89" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" s="1"/>
+      <c r="G89" s="25"/>
+      <c r="H89" s="25"/>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C90" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F90" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G90" s="25"/>
+      <c r="H90" s="25"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C91" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F91" s="1"/>
+      <c r="G91" s="25"/>
+      <c r="H91" s="25"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="C92" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F92" s="1"/>
+      <c r="G92" s="25"/>
+      <c r="H92" s="25"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C93" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D93" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E93" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="F93" s="1"/>
+      <c r="G93" s="25"/>
+      <c r="H93" s="25"/>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="C94" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F94" s="1">
+        <v>5000</v>
+      </c>
+      <c r="G94" s="25"/>
+      <c r="H94" s="25"/>
+    </row>
+    <row r="95" spans="1:8">
+      <c r="A95" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="C95" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="E95" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="F95" s="1"/>
+      <c r="G95" s="25"/>
+      <c r="H95" s="25"/>
+    </row>
+    <row r="96" spans="1:8">
+      <c r="A96" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C96" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F96" s="1">
+        <v>7000</v>
+      </c>
+      <c r="G96" s="25"/>
+      <c r="H96" s="25"/>
+    </row>
+    <row r="97" spans="1:8">
+      <c r="A97" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="C97" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F97" s="1"/>
+      <c r="G97" s="25"/>
+      <c r="H97" s="25"/>
+    </row>
+    <row r="98" spans="1:8">
+      <c r="A98" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C98" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F98" s="1"/>
+      <c r="G98" s="25"/>
+      <c r="H98" s="25"/>
+    </row>
+    <row r="99" spans="1:8">
+      <c r="A99" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="C99" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F99" s="1"/>
+      <c r="G99" s="25"/>
+      <c r="H99" s="25"/>
+    </row>
+    <row r="100" spans="1:8">
+      <c r="A100" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="C100" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F100" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G100" s="25"/>
+      <c r="H100" s="25"/>
+    </row>
+    <row r="101" spans="1:8">
+      <c r="A101" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C101" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F101" s="1"/>
+      <c r="G101" s="25"/>
+      <c r="H101" s="25"/>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="C102" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F102" s="1"/>
+      <c r="G102" s="25"/>
+      <c r="H102" s="25"/>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C103" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F103" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G103" s="25"/>
+      <c r="H103" s="25"/>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C104" s="26" t="s">
+        <v>563</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F104" s="1"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -19777,8 +21157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D16" sqref="D16:E18"/>
+    <sheetView topLeftCell="A73" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21580,8 +22960,8 @@
   </sheetPr>
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A16" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D19" sqref="D19:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23312,8 +24692,8 @@
   </sheetPr>
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
running the failed 5 scenarios
</commit_message>
<xml_diff>
--- a/TestDataAndResults/Run1/SophieAutomation.xlsx
+++ b/TestDataAndResults/Run1/SophieAutomation.xlsx
@@ -1,40 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF248D4E-9299-4D7D-888E-334D34934B3B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9180DD22-6A90-4315-8707-3D8F0866EA58}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView tabRatio="500" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="DriverSheet" sheetId="2" r:id="rId1"/>
-    <sheet name="VerifyCSVForExistingVersion" sheetId="3" r:id="rId2"/>
-    <sheet name="VerifyCSVForNewVersion" sheetId="4" r:id="rId3"/>
-    <sheet name="VerifyChannelSelection" sheetId="23" r:id="rId4"/>
-    <sheet name="VerifyIHDeleted" sheetId="20" r:id="rId5"/>
-    <sheet name="VerifyDeleteOffer" sheetId="5" r:id="rId6"/>
-    <sheet name="RenameOffer" sheetId="21" r:id="rId7"/>
-    <sheet name="VerifyEventAPI" sheetId="6" r:id="rId8"/>
-    <sheet name="PickBestChannel" sheetId="24" r:id="rId9"/>
-    <sheet name="VerifyRealtimeSpineAPI" sheetId="7" r:id="rId10"/>
-    <sheet name="RealtimeSpineWithNewProperty" sheetId="10" r:id="rId11"/>
-    <sheet name="EmailTempWithNewAttribute" sheetId="11" r:id="rId12"/>
-    <sheet name="MicrositeTempWithExistingAttrib" sheetId="12" r:id="rId13"/>
-    <sheet name="OBCCTempWithExistingAttrib" sheetId="17" r:id="rId14"/>
-    <sheet name="VerifyDBForNewAgreementModel" sheetId="13" r:id="rId15"/>
-    <sheet name="VerifyAgreementClassFornewProp" sheetId="14" r:id="rId16"/>
-    <sheet name="VerifyDiscardVersioIsSuccessful" sheetId="15" r:id="rId17"/>
-    <sheet name="EnsureRollbackIsSuccessful" sheetId="16" r:id="rId18"/>
-    <sheet name="AdpativeModelForUnsubscribe" sheetId="18" r:id="rId19"/>
-    <sheet name="SingleChannelOn" sheetId="22" r:id="rId20"/>
-    <sheet name="BatchDecisionOutputValidations" sheetId="8" r:id="rId21"/>
-    <sheet name="CheckLists" sheetId="9" r:id="rId22"/>
+    <sheet name="DriverSheet" r:id="rId1" sheetId="2"/>
+    <sheet name="VerifyCSVForExistingVersion" r:id="rId2" sheetId="3"/>
+    <sheet name="VerifyCSVForNewVersion" r:id="rId3" sheetId="4"/>
+    <sheet name="VerifyChannelSelection" r:id="rId4" sheetId="23"/>
+    <sheet name="VerifyIHDeleted" r:id="rId5" sheetId="20"/>
+    <sheet name="VerifyDeleteOffer" r:id="rId6" sheetId="5"/>
+    <sheet name="RenameOffer" r:id="rId7" sheetId="21"/>
+    <sheet name="VerifyEventAPI" r:id="rId8" sheetId="6"/>
+    <sheet name="PickBestChannel" r:id="rId9" sheetId="24"/>
+    <sheet name="VerifyRealtimeSpineAPI" r:id="rId10" sheetId="7"/>
+    <sheet name="RealtimeSpineWithNewProperty" r:id="rId11" sheetId="10"/>
+    <sheet name="EmailTempWithNewAttribute" r:id="rId12" sheetId="11"/>
+    <sheet name="MicrositeTempWithExistingAttrib" r:id="rId13" sheetId="12"/>
+    <sheet name="OBCCTempWithExistingAttrib" r:id="rId14" sheetId="17"/>
+    <sheet name="VerifyDBForNewAgreementModel" r:id="rId15" sheetId="13"/>
+    <sheet name="VerifyAgreementClassFornewProp" r:id="rId16" sheetId="14"/>
+    <sheet name="VerifyDiscardVersioIsSuccessful" r:id="rId17" sheetId="15"/>
+    <sheet name="EnsureRollbackIsSuccessful" r:id="rId18" sheetId="16"/>
+    <sheet name="AdpativeModelForUnsubscribe" r:id="rId19" sheetId="18"/>
+    <sheet name="SingleChannelOn" r:id="rId20" sheetId="22"/>
+    <sheet name="BatchDecisionOutputValidations" r:id="rId21" sheetId="8"/>
+    <sheet name="CheckLists" r:id="rId22" sheetId="9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6584" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6677" uniqueCount="638">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1871,12 +1871,6 @@
     <t>SMSUK</t>
   </si>
   <si>
-    <t>override the offer</t>
-  </si>
-  <si>
-    <t>increase the weight</t>
-  </si>
-  <si>
     <t>txtSearchOnEligbileOffers</t>
   </si>
   <si>
@@ -1901,76 +1895,79 @@
     <t>Verifying the selected channels in UI</t>
   </si>
   <si>
+    <t>quit browser</t>
+  </si>
+  <si>
+    <t>Below scenario is to ensure the pick best channel scenario for the channel heirarchy</t>
+  </si>
+  <si>
+    <t>Pick best channel Scenario</t>
+  </si>
+  <si>
+    <t>webTableForOffer</t>
+  </si>
+  <si>
+    <t>btnCustomerChannels</t>
+  </si>
+  <si>
+    <t>click on customer channels</t>
+  </si>
+  <si>
+    <t>PickBestChannel</t>
+  </si>
+  <si>
+    <t>Verifying the pick best channel with channel heirarchy</t>
+  </si>
+  <si>
+    <t>webTableForChannel</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>btnSaveChannelHi</t>
+  </si>
+  <si>
+    <t>changeChannelPriorityIfRequired</t>
+  </si>
+  <si>
+    <t>PickBestOffer</t>
+  </si>
+  <si>
+    <t>chkOBCC2</t>
+  </si>
+  <si>
+    <t>chkPickBest</t>
+  </si>
+  <si>
+    <t>rdnChannelHi</t>
+  </si>
+  <si>
+    <t>tabOBCC</t>
+  </si>
+  <si>
+    <t>ddnOBCCTemplate</t>
+  </si>
+  <si>
+    <t>Sophie Default OutboundCC</t>
+  </si>
+  <si>
+    <t>ddnOBCCSubChannel</t>
+  </si>
+  <si>
+    <t>OutboundCCUK</t>
+  </si>
+  <si>
+    <t>verifyEligibleChannelForOfferInDB</t>
+  </si>
+  <si>
+    <t>select distinct channel from interaction_history_v where associatedoffer='PickBestOffer'</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>quit browser</t>
-  </si>
-  <si>
-    <t>Below scenario is to ensure the pick best channel scenario for the channel heirarchy</t>
-  </si>
-  <si>
-    <t>Pick best channel Scenario</t>
-  </si>
-  <si>
-    <t>webTableForOffer</t>
-  </si>
-  <si>
-    <t>btnCustomerChannels</t>
-  </si>
-  <si>
-    <t>click on customer channels</t>
-  </si>
-  <si>
-    <t>PickBestChannel</t>
-  </si>
-  <si>
-    <t>Verifying the pick best channel with channel heirarchy</t>
-  </si>
-  <si>
-    <t>webTableForChannel</t>
-  </si>
-  <si>
-    <t>EMAIL</t>
-  </si>
-  <si>
-    <t>btnSaveChannelHi</t>
-  </si>
-  <si>
-    <t>changeChannelPriorityIfRequired</t>
-  </si>
-  <si>
-    <t>PickBestOffer</t>
-  </si>
-  <si>
-    <t>chkOBCC2</t>
-  </si>
-  <si>
-    <t>chkPickBest</t>
-  </si>
-  <si>
-    <t>rdnChannelHi</t>
-  </si>
-  <si>
-    <t>tabOBCC</t>
-  </si>
-  <si>
-    <t>ddnOBCCTemplate</t>
-  </si>
-  <si>
-    <t>Sophie Default OutboundCC</t>
-  </si>
-  <si>
-    <t>ddnOBCCSubChannel</t>
-  </si>
-  <si>
-    <t>OutboundCCUK</t>
-  </si>
-  <si>
-    <t>verifyEligibleChannelForOfferInDB</t>
-  </si>
-  <si>
-    <t>select distinct channel from interaction_history_v where associatedoffer='PickBestOffer'</t>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -2209,82 +2206,82 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyBorder="0" applyProtection="0" borderId="0" fillId="0" fontId="4" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="10" fillId="4" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{58C6B9B9-44EF-4FF6-B4E2-0E7E1176543B}"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2369,10 +2366,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2407,7 +2404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2459,7 +2456,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -2570,21 +2567,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2601,7 +2598,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2653,31 +2650,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="2" customWidth="1"/>
-    <col min="6" max="1025" width="9.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="70.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="19.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="24.42578125" collapsed="true"/>
+    <col min="6" max="1025" customWidth="true" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="1" s="3" spans="1:5">
       <c r="A1" s="40" t="s">
         <v>4</v>
       </c>
@@ -2686,7 +2683,7 @@
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="2" s="3" spans="1:5">
       <c r="A2" s="41" t="s">
         <v>5</v>
       </c>
@@ -2695,14 +2692,14 @@
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="3" s="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="14.25">
+    <row customFormat="1" ht="14.25" r="4" s="6" spans="1:5">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
@@ -2730,7 +2727,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -2745,7 +2742,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -2760,7 +2757,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -2775,7 +2772,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2790,7 +2787,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -2805,7 +2802,7 @@
         <v>360</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -2820,7 +2817,7 @@
         <v>409</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -2835,7 +2832,7 @@
         <v>446</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -2850,7 +2847,7 @@
         <v>459</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -2865,7 +2862,7 @@
         <v>477</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -2880,7 +2877,7 @@
         <v>504</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E15" s="1"/>
     </row>
@@ -2895,7 +2892,7 @@
         <v>540</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E16" s="1"/>
     </row>
@@ -2910,7 +2907,7 @@
         <v>541</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E17" s="1"/>
     </row>
@@ -2925,7 +2922,7 @@
         <v>552</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -2934,13 +2931,13 @@
         <v>518</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>615</v>
+        <v>636</v>
       </c>
       <c r="E19" s="1"/>
     </row>
@@ -2949,10 +2946,10 @@
         <v>538</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>13</v>
@@ -2964,33 +2961,33 @@
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -4470,17 +4467,17 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F1A5F4-9176-42F8-9D13-5A98D8683A92}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32F1A5F4-9176-42F8-9D13-5A98D8683A92}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:F21"/>
@@ -4488,11 +4485,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -6552,16 +6549,16 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162B974F-EC20-4DA5-9D9F-A5ACD05AB2C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162B974F-EC20-4DA5-9D9F-A5ACD05AB2C7}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="F68" sqref="F68"/>
@@ -6569,12 +6566,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8232,13 +8229,13 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CE6C41-C6E4-4D12-92D1-A13E0879FD5B}">
-  <dimension ref="A1:H78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CE6C41-C6E4-4D12-92D1-A13E0879FD5B}">
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="E80" sqref="E80"/>
@@ -8246,14 +8243,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="36.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -9863,16 +9860,16 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DC9284-1E00-457F-9E32-CE2FA20C3859}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DC9284-1E00-457F-9E32-CE2FA20C3859}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
@@ -9880,12 +9877,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -10312,27 +10309,27 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92316FED-85B2-43F2-9827-12AFBA752185}">
-  <dimension ref="A1:H53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92316FED-85B2-43F2-9827-12AFBA752185}">
+  <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44:E44"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="40.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="40.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="40.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -11426,13 +11423,13 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDE53E4-1746-48CE-AB4D-617AE971D39B}">
-  <dimension ref="A1:H66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDE53E4-1746-48CE-AB4D-617AE971D39B}">
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
@@ -11440,12 +11437,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="44.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -12813,13 +12810,13 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B88A9-98DC-469F-B6A8-72D4BD0DF47F}">
-  <dimension ref="A1:H98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B88A9-98DC-469F-B6A8-72D4BD0DF47F}">
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView topLeftCell="B86" workbookViewId="0">
       <selection activeCell="E96" sqref="E96"/>
@@ -12827,13 +12824,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.42578125" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -14879,30 +14876,30 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D209F-F23A-4BBD-9C0E-30D3275A1C3F}">
-  <dimension ref="A1:H117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D209F-F23A-4BBD-9C0E-30D3275A1C3F}">
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C116" sqref="C116:F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29.25" customHeight="1">
+    <row customHeight="1" ht="29.25" r="1" spans="1:8">
       <c r="A1" s="44" t="s">
         <v>497</v>
       </c>
@@ -17343,26 +17340,26 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB81825B-AC84-43BA-896B-AD045DB7862F}">
-  <dimension ref="A1:H41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB81825B-AC84-43BA-896B-AD045DB7862F}">
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -18205,6 +18202,48 @@
       <c r="G41" s="25"/>
       <c r="H41" s="25"/>
     </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>450</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>450</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
@@ -18212,28 +18251,28 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A40" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
-    <col min="6" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -19227,7 +19266,7 @@
         <v>41</v>
       </c>
       <c r="F49" s="1">
-        <v>30000</v>
+        <v>90000</v>
       </c>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -19258,13 +19297,13 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A4A3E8-7749-4CD2-9C58-29CEA684BAD6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A4A3E8-7749-4CD2-9C58-29CEA684BAD6}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19273,29 +19312,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -19494,24 +19533,24 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A2:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A2:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2">
@@ -19531,28 +19570,28 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="D57" sqref="D57:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="34.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="7" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -21020,14 +21059,14 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57E7C9-DCBE-422B-912B-E6D243214D2D}">
-  <dimension ref="A1:H57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE57E7C9-DCBE-422B-912B-E6D243214D2D}">
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D23" sqref="D23:F41"/>
@@ -21035,12 +21074,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -21057,7 +21096,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="42" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -21458,7 +21497,7 @@
         <v>70</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9"/>
@@ -21480,7 +21519,7 @@
         <v>70</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="9"/>
@@ -21626,7 +21665,7 @@
         <v>70</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
@@ -21935,7 +21974,7 @@
         <v>158</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>34</v>
@@ -21944,7 +21983,7 @@
         <v>165</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
@@ -22005,7 +22044,7 @@
         <v>34</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F47" s="25" t="s">
         <v>263</v>
@@ -22207,7 +22246,7 @@
         <v>335</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>34</v>
@@ -22226,13 +22265,13 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440AE6C1-8303-4801-938E-D5D89C6CD179}">
-  <dimension ref="A1:H33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{440AE6C1-8303-4801-938E-D5D89C6CD179}">
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D33" sqref="D33:E33"/>
@@ -22240,14 +22279,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -22921,28 +22960,28 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A44" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="D54" sqref="D54:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" customWidth="1"/>
-    <col min="9" max="1025" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="31.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="9" max="1025" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -24051,27 +24090,27 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFAFDA0-4A55-4936-A3DC-B19DEB90A342}">
-  <dimension ref="A1:H106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFAFDA0-4A55-4936-A3DC-B19DEB90A342}">
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56:F65"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105:E106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -25193,7 +25232,7 @@
         <v>555</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>553</v>
@@ -26277,28 +26316,28 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H93"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:F31"/>
+    <sheetView topLeftCell="A62" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="A71" sqref="A71:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.140625" customWidth="1"/>
-    <col min="6" max="6" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="29.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="8" max="1025" customWidth="true" width="8.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -27761,22 +27800,20 @@
       <c r="A71" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>155</v>
+      <c r="B71" s="15" t="s">
+        <v>159</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>605</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G71" s="21"/>
+        <v>98</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E71" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
       <c r="H71" s="9"/>
     </row>
     <row r="72" spans="1:8">
@@ -27784,41 +27821,39 @@
         <v>17</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>606</v>
+        <v>159</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G72" s="21"/>
+        <v>45</v>
+      </c>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E73" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
+      <c r="B73" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="20" t="s">
+        <v>496</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
       <c r="H73" s="9"/>
     </row>
     <row r="74" spans="1:8">
@@ -27826,19 +27861,19 @@
         <v>17</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
+        <v>40</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
       <c r="H74" s="9"/>
     </row>
     <row r="75" spans="1:8">
@@ -27854,10 +27889,12 @@
       <c r="D75" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E75" s="20" t="s">
-        <v>496</v>
-      </c>
-      <c r="F75" s="1"/>
+      <c r="E75" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F75" s="1">
+        <v>7000</v>
+      </c>
       <c r="G75" s="1"/>
       <c r="H75" s="9"/>
     </row>
@@ -27866,16 +27903,16 @@
         <v>17</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>252</v>
+        <v>105</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -27886,20 +27923,18 @@
         <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D77" s="20" t="s">
-        <v>34</v>
+        <v>120</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F77" s="1">
-        <v>7000</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="9"/>
     </row>
@@ -27908,18 +27943,20 @@
         <v>17</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>105</v>
+        <v>40</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F78" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="F78" s="1">
+        <v>30000</v>
+      </c>
       <c r="G78" s="1"/>
       <c r="H78" s="9"/>
     </row>
@@ -27928,18 +27965,20 @@
         <v>17</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>120</v>
+        <v>201</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>121</v>
+        <v>2</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F79" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>202</v>
+      </c>
       <c r="G79" s="1"/>
       <c r="H79" s="9"/>
     </row>
@@ -27951,7 +27990,7 @@
         <v>122</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>40</v>
+        <v>289</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>34</v>
@@ -27960,7 +27999,7 @@
         <v>41</v>
       </c>
       <c r="F80" s="1">
-        <v>30000</v>
+        <v>180000</v>
       </c>
       <c r="G80" s="1"/>
       <c r="H80" s="9"/>
@@ -27973,17 +28012,15 @@
         <v>122</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>201</v>
+        <v>320</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>2</v>
+        <v>321</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>202</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="9"/>
     </row>
@@ -27995,17 +28032,15 @@
         <v>122</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>289</v>
+        <v>323</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>34</v>
+        <v>322</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F82" s="1">
-        <v>180000</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="9"/>
     </row>
@@ -28017,15 +28052,17 @@
         <v>122</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>320</v>
+        <v>64</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>321</v>
+        <v>34</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F83" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="F83" s="1">
+        <v>5000</v>
+      </c>
       <c r="G83" s="1"/>
       <c r="H83" s="9"/>
     </row>
@@ -28037,10 +28074,10 @@
         <v>122</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>45</v>
@@ -28057,7 +28094,7 @@
         <v>122</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>64</v>
+        <v>328</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>34</v>
@@ -28066,7 +28103,7 @@
         <v>41</v>
       </c>
       <c r="F85" s="1">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="G85" s="1"/>
       <c r="H85" s="9"/>
@@ -28079,10 +28116,10 @@
         <v>122</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>324</v>
+        <v>605</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>45</v>
@@ -28099,16 +28136,16 @@
         <v>122</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>34</v>
+        <v>605</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F87" s="1">
-        <v>3000</v>
+        <v>70</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>194</v>
       </c>
       <c r="G87" s="1"/>
       <c r="H87" s="9"/>
@@ -28121,15 +28158,17 @@
         <v>122</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>328</v>
+        <v>64</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>607</v>
+        <v>34</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="F88" s="1">
+        <v>5000</v>
+      </c>
       <c r="G88" s="1"/>
       <c r="H88" s="9"/>
     </row>
@@ -28141,17 +28180,15 @@
         <v>122</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>607</v>
+        <v>308</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>194</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="9"/>
     </row>
@@ -28163,18 +28200,20 @@
         <v>122</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>64</v>
+        <v>203</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F90" s="1">
-        <v>5000</v>
-      </c>
-      <c r="G90" s="1"/>
+        <v>204</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="H90" s="9"/>
     </row>
     <row r="91" spans="1:8">
@@ -28182,64 +28221,20 @@
         <v>17</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>327</v>
+        <v>124</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>308</v>
+        <v>34</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="9"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H92" s="9"/>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -28248,27 +28243,27 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup firstPageNumber="0" horizontalDpi="300" orientation="portrait" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D9D972-BC3C-4059-B86B-F0917555266F}">
-  <dimension ref="A1:H84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93D9D972-BC3C-4059-B86B-F0917555266F}">
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView topLeftCell="C73" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="81.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -28295,7 +28290,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="42" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
@@ -28351,7 +28346,9 @@
         <v>34</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
@@ -28373,7 +28370,9 @@
         <v>34</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
@@ -28395,7 +28394,9 @@
         <v>174</v>
       </c>
       <c r="G7" s="14"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
@@ -28415,7 +28416,9 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
@@ -28437,7 +28440,9 @@
         <v>161</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
@@ -28457,7 +28462,9 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
@@ -28479,7 +28486,9 @@
         <v>162</v>
       </c>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -28501,7 +28510,9 @@
         <v>2</v>
       </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -28523,7 +28534,9 @@
         <v>162</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -28543,7 +28556,9 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
@@ -28565,7 +28580,9 @@
         <v>1</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
@@ -28587,7 +28604,9 @@
         <v>5000</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
@@ -28607,7 +28626,9 @@
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
@@ -28627,7 +28648,9 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
@@ -28647,7 +28670,9 @@
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
@@ -28667,7 +28692,9 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
+      <c r="H20" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
@@ -28689,7 +28716,9 @@
         <v>162</v>
       </c>
       <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="H21" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
@@ -28711,7 +28740,9 @@
         <v>2</v>
       </c>
       <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
+      <c r="H22" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
@@ -28731,7 +28762,9 @@
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
+      <c r="H23" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
@@ -28751,7 +28784,9 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
+      <c r="H24" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
@@ -28773,7 +28808,9 @@
         <v>10000</v>
       </c>
       <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
+      <c r="H25" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
@@ -28793,7 +28830,9 @@
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
+      <c r="H26" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
@@ -28812,10 +28851,12 @@
         <v>70</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
+      <c r="H27" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
@@ -28834,10 +28875,12 @@
         <v>70</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
+      <c r="H28" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
@@ -28857,7 +28900,9 @@
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
+      <c r="H29" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -28879,7 +28924,9 @@
         <v>3000</v>
       </c>
       <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
+      <c r="H30" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -28889,17 +28936,19 @@
         <v>97</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F31" s="25"/>
       <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
+      <c r="H31" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
@@ -28909,19 +28958,21 @@
         <v>97</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D32" s="26" t="s">
         <v>621</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="E32" s="26" t="s">
         <v>624</v>
       </c>
-      <c r="E32" s="26" t="s">
-        <v>627</v>
-      </c>
       <c r="F32" s="26" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
+      <c r="H32" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
@@ -28931,17 +28982,19 @@
         <v>97</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E33" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F33" s="25"/>
       <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
+      <c r="H33" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
@@ -28951,7 +29004,7 @@
         <v>97</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>78</v>
@@ -28961,7 +29014,9 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
+      <c r="H34" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
@@ -28971,7 +29026,7 @@
         <v>97</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>34</v>
@@ -28983,7 +29038,9 @@
         <v>3000</v>
       </c>
       <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
+      <c r="H35" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
@@ -28993,7 +29050,7 @@
         <v>97</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>78</v>
@@ -29003,7 +29060,9 @@
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
+      <c r="H36" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
@@ -29013,7 +29072,7 @@
         <v>97</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>34</v>
@@ -29025,7 +29084,9 @@
         <v>3000</v>
       </c>
       <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
+      <c r="H37" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
@@ -29035,7 +29096,7 @@
         <v>97</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>134</v>
@@ -29045,7 +29106,9 @@
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
+      <c r="H38" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
@@ -29055,7 +29118,7 @@
         <v>97</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>136</v>
@@ -29064,10 +29127,12 @@
         <v>70</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
+      <c r="H39" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
@@ -29077,7 +29142,7 @@
         <v>97</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>139</v>
@@ -29089,7 +29154,9 @@
         <v>43525</v>
       </c>
       <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
+      <c r="H40" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
@@ -29099,7 +29166,7 @@
         <v>97</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>141</v>
@@ -29111,7 +29178,9 @@
         <v>45719</v>
       </c>
       <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
+      <c r="H41" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
@@ -29121,7 +29190,7 @@
         <v>97</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>143</v>
@@ -29131,7 +29200,9 @@
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
+      <c r="H42" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
@@ -29141,7 +29212,7 @@
         <v>97</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>429</v>
@@ -29153,7 +29224,9 @@
         <v>430</v>
       </c>
       <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
+      <c r="H43" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
@@ -29163,7 +29236,7 @@
         <v>97</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>431</v>
@@ -29173,7 +29246,9 @@
       </c>
       <c r="F44" s="36"/>
       <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
+      <c r="H44" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
@@ -29183,7 +29258,7 @@
         <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>432</v>
@@ -29195,7 +29270,9 @@
         <v>433</v>
       </c>
       <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
+      <c r="H45" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
@@ -29205,7 +29282,7 @@
         <v>97</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>436</v>
@@ -29215,7 +29292,9 @@
       </c>
       <c r="F46" s="36"/>
       <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
+      <c r="H46" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
@@ -29225,7 +29304,7 @@
         <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>438</v>
@@ -29235,7 +29314,9 @@
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
+      <c r="H47" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
@@ -29245,7 +29326,7 @@
         <v>97</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>441</v>
@@ -29255,7 +29336,9 @@
       </c>
       <c r="F48" s="36"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
+      <c r="H48" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
@@ -29265,17 +29348,19 @@
         <v>97</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>82</v>
       </c>
       <c r="F49" s="36"/>
       <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
+      <c r="H49" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
@@ -29285,17 +29370,19 @@
         <v>97</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>82</v>
       </c>
       <c r="F50" s="36"/>
       <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
+      <c r="H50" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -29305,17 +29392,19 @@
         <v>97</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F51" s="36"/>
       <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
+      <c r="H51" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
@@ -29325,7 +29414,7 @@
         <v>97</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>143</v>
@@ -29335,7 +29424,9 @@
       </c>
       <c r="F52" s="36"/>
       <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
+      <c r="H52" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
@@ -29345,7 +29436,7 @@
         <v>97</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>145</v>
@@ -29355,7 +29446,9 @@
       </c>
       <c r="F53" s="9"/>
       <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
+      <c r="H53" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
@@ -29365,7 +29458,7 @@
         <v>97</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>147</v>
@@ -29377,7 +29470,9 @@
         <v>149</v>
       </c>
       <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
+      <c r="H54" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
@@ -29387,7 +29482,7 @@
         <v>97</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>34</v>
@@ -29399,7 +29494,9 @@
         <v>3000</v>
       </c>
       <c r="G55" s="25"/>
-      <c r="H55" s="25"/>
+      <c r="H55" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
@@ -29409,7 +29506,7 @@
         <v>97</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>585</v>
@@ -29421,7 +29518,9 @@
         <v>586</v>
       </c>
       <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
+      <c r="H56" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
@@ -29431,7 +29530,7 @@
         <v>97</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>151</v>
@@ -29441,7 +29540,9 @@
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="25"/>
+      <c r="H57" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
@@ -29451,7 +29552,7 @@
         <v>97</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>153</v>
@@ -29463,7 +29564,9 @@
         <v>154</v>
       </c>
       <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
+      <c r="H58" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
@@ -29473,7 +29576,7 @@
         <v>97</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>34</v>
@@ -29485,7 +29588,9 @@
         <v>3000</v>
       </c>
       <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
+      <c r="H59" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
@@ -29495,7 +29600,7 @@
         <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>584</v>
@@ -29507,7 +29612,9 @@
         <v>583</v>
       </c>
       <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
+      <c r="H60" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
@@ -29517,7 +29624,7 @@
         <v>97</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D61" s="26" t="s">
         <v>195</v>
@@ -29527,7 +29634,9 @@
       </c>
       <c r="F61" s="25"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
+      <c r="H61" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
@@ -29537,7 +29646,7 @@
         <v>97</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D62" s="26" t="s">
         <v>196</v>
@@ -29549,7 +29658,9 @@
         <v>197</v>
       </c>
       <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
+      <c r="H62" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
@@ -29559,7 +29670,7 @@
         <v>97</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>34</v>
@@ -29571,7 +29682,9 @@
         <v>3000</v>
       </c>
       <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
+      <c r="H63" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
@@ -29581,7 +29694,7 @@
         <v>97</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D64" s="26" t="s">
         <v>603</v>
@@ -29593,7 +29706,9 @@
         <v>604</v>
       </c>
       <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
+      <c r="H64" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
@@ -29603,17 +29718,19 @@
         <v>100</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="E65" s="26" t="s">
         <v>45</v>
       </c>
       <c r="F65" s="25"/>
       <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
+      <c r="H65" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
@@ -29623,19 +29740,21 @@
         <v>103</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D66" s="26" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="E66" s="26" t="s">
         <v>148</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="G66" s="25"/>
-      <c r="H66" s="25"/>
+      <c r="H66" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
@@ -29645,7 +29764,7 @@
         <v>104</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>34</v>
@@ -29657,7 +29776,9 @@
         <v>3000</v>
       </c>
       <c r="G67" s="25"/>
-      <c r="H67" s="25"/>
+      <c r="H67" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
@@ -29667,19 +29788,21 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D68" s="26" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="E68" s="26" t="s">
         <v>148</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="G68" s="25"/>
-      <c r="H68" s="25"/>
+      <c r="H68" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
@@ -29689,7 +29812,7 @@
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>143</v>
@@ -29699,7 +29822,9 @@
       </c>
       <c r="F69" s="25"/>
       <c r="G69" s="25"/>
-      <c r="H69" s="25"/>
+      <c r="H69" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
@@ -29709,7 +29834,7 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>34</v>
@@ -29721,7 +29846,9 @@
         <v>5000</v>
       </c>
       <c r="G70" s="25"/>
-      <c r="H70" s="25"/>
+      <c r="H70" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
@@ -29731,7 +29858,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>78</v>
@@ -29741,7 +29868,9 @@
       </c>
       <c r="F71" s="25"/>
       <c r="G71" s="25"/>
-      <c r="H71" s="25"/>
+      <c r="H71" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
@@ -29751,7 +29880,7 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>34</v>
@@ -29760,10 +29889,12 @@
         <v>550</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G72" s="25"/>
-      <c r="H72" s="25"/>
+      <c r="H72" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
@@ -29773,19 +29904,21 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>553</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="G73" s="25"/>
-      <c r="H73" s="25"/>
+      <c r="H73" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
@@ -29795,7 +29928,7 @@
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>34</v>
@@ -29807,7 +29940,9 @@
         <v>3000</v>
       </c>
       <c r="G74" s="25"/>
-      <c r="H74" s="25"/>
+      <c r="H74" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
@@ -29817,7 +29952,7 @@
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>99</v>
@@ -29827,7 +29962,9 @@
       </c>
       <c r="F75" s="1"/>
       <c r="G75" s="25"/>
-      <c r="H75" s="25"/>
+      <c r="H75" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
@@ -29837,7 +29974,7 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>102</v>
@@ -29847,7 +29984,9 @@
       </c>
       <c r="F76" s="1"/>
       <c r="G76" s="25"/>
-      <c r="H76" s="25"/>
+      <c r="H76" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
@@ -29857,7 +29996,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>34</v>
@@ -29867,7 +30006,9 @@
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="25"/>
-      <c r="H77" s="25"/>
+      <c r="H77" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
@@ -29877,7 +30018,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>276</v>
@@ -29887,7 +30028,9 @@
       </c>
       <c r="F78" s="1"/>
       <c r="G78" s="25"/>
-      <c r="H78" s="25"/>
+      <c r="H78" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
@@ -29897,7 +30040,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>34</v>
@@ -29909,7 +30052,9 @@
         <v>7000</v>
       </c>
       <c r="G79" s="25"/>
-      <c r="H79" s="25"/>
+      <c r="H79" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
@@ -29919,7 +30064,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>106</v>
@@ -29929,7 +30074,9 @@
       </c>
       <c r="F80" s="1"/>
       <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
+      <c r="H80" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="1" t="s">
@@ -29939,7 +30086,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>121</v>
@@ -29949,7 +30096,9 @@
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="25"/>
-      <c r="H81" s="25"/>
+      <c r="H81" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="1" t="s">
@@ -29959,7 +30108,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>34</v>
@@ -29971,7 +30120,9 @@
         <v>30000</v>
       </c>
       <c r="G82" s="25"/>
-      <c r="H82" s="25"/>
+      <c r="H82" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
@@ -29981,7 +30132,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>2</v>
@@ -29993,7 +30144,9 @@
         <v>202</v>
       </c>
       <c r="G83" s="25"/>
-      <c r="H83" s="25"/>
+      <c r="H83" s="25" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="1" t="s">
@@ -30003,21 +30156,87 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="D84" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E84" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F84" s="1">
+        <v>60000</v>
+      </c>
+      <c r="G84" s="25"/>
+      <c r="H84" s="25" t="s">
         <v>637</v>
       </c>
-      <c r="F84" s="25" t="s">
-        <v>638</v>
-      </c>
-      <c r="G84" s="25" t="s">
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" s="26" t="s">
+        <v>634</v>
+      </c>
+      <c r="F85" s="25" t="s">
+        <v>635</v>
+      </c>
+      <c r="G85" s="25" t="s">
         <v>263</v>
       </c>
-      <c r="H84" s="25"/>
+      <c r="H85" s="25"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F86" s="25">
+        <v>3000</v>
+      </c>
+      <c r="G86" s="25"/>
+      <c r="H86" s="25"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F87" s="25"/>
+      <c r="G87" s="25"/>
+      <c r="H87" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -30026,6 +30245,6 @@
     <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>